<commit_message>
Finalizado metodos de NBA, posiciones sacadas
</commit_message>
<xml_diff>
--- a/NBA.xlsx
+++ b/NBA.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="46">
   <si>
     <t>Nombre</t>
   </si>
@@ -19,7 +19,7 @@
     <t>Equipo</t>
   </si>
   <si>
-    <t>Estatura</t>
+    <t>Edad</t>
   </si>
   <si>
     <t>Salario</t>
@@ -41,9 +41,6 @@
   </si>
   <si>
     <t>Puntos</t>
-  </si>
-  <si>
-    <t>Edad</t>
   </si>
   <si>
     <t>Puntuacion</t>
@@ -212,23 +209,20 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="7">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
     <xf borderId="1" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment readingOrder="0"/>
     </xf>
+    <xf borderId="1" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment readingOrder="0"/>
+    </xf>
     <xf borderId="2" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment readingOrder="0"/>
     </xf>
-    <xf borderId="1" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment readingOrder="0"/>
-    </xf>
     <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="3" numFmtId="3" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
       <alignment readingOrder="0"/>
     </xf>
     <xf borderId="1" fillId="0" fontId="2" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
@@ -265,10 +259,10 @@
       <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D1" s="2" t="s">
         <v>3</v>
       </c>
       <c r="E1" s="1" t="s">
@@ -289,28 +283,22 @@
       <c r="J1" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="K1" s="2" t="s">
+      <c r="K1" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="L1" s="2" t="s">
         <v>10</v>
-      </c>
-      <c r="L1" s="3" t="s">
-        <v>11</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="B2" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="B2" s="4" t="s">
+      <c r="E2" s="4" t="s">
         <v>13</v>
-      </c>
-      <c r="C2" s="4">
-        <v>170.0</v>
-      </c>
-      <c r="D2" s="5">
-        <v>200000.0</v>
-      </c>
-      <c r="E2" s="4" t="s">
-        <v>14</v>
       </c>
       <c r="F2" s="4">
         <v>5.1</v>
@@ -330,26 +318,20 @@
       <c r="K2" s="4">
         <v>28.0</v>
       </c>
-      <c r="L2" s="3">
+      <c r="L2" s="2">
         <f t="shared" ref="L2:L13" si="1">IFS(E2="Base",SUM(I2,J2,G2),E2="Alero",SUM(H2,J2,F2),E2="Pivot",SUM(F2,J2,I2),E2="Escolta",SUM(H2,J2,G2))</f>
         <v>35.7</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="B3" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="B3" s="4" t="s">
+      <c r="E3" s="4" t="s">
         <v>16</v>
-      </c>
-      <c r="C3" s="4">
-        <v>190.0</v>
-      </c>
-      <c r="D3" s="5">
-        <v>180000.0</v>
-      </c>
-      <c r="E3" s="4" t="s">
-        <v>17</v>
       </c>
       <c r="F3" s="4">
         <v>11.9</v>
@@ -369,26 +351,20 @@
       <c r="K3" s="4">
         <v>24.0</v>
       </c>
-      <c r="L3" s="6">
+      <c r="L3" s="5">
         <f t="shared" si="1"/>
         <v>44.3</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="B4" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="B4" s="4" t="s">
+      <c r="E4" s="4" t="s">
         <v>19</v>
-      </c>
-      <c r="C4" s="4">
-        <v>182.0</v>
-      </c>
-      <c r="D4" s="5">
-        <v>190000.0</v>
-      </c>
-      <c r="E4" s="4" t="s">
-        <v>20</v>
       </c>
       <c r="F4" s="4">
         <v>7.8</v>
@@ -408,26 +384,20 @@
       <c r="K4" s="4">
         <v>27.0</v>
       </c>
-      <c r="L4" s="6">
+      <c r="L4" s="5">
         <f t="shared" si="1"/>
         <v>37</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="B5" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="B5" s="4" t="s">
-        <v>22</v>
-      </c>
-      <c r="C5" s="4">
-        <v>168.0</v>
-      </c>
-      <c r="D5" s="5">
-        <v>140000.0</v>
-      </c>
       <c r="E5" s="4" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="F5" s="4">
         <v>9.6</v>
@@ -447,26 +417,20 @@
       <c r="K5" s="4">
         <v>29.0</v>
       </c>
-      <c r="L5" s="6">
+      <c r="L5" s="5">
         <f t="shared" si="1"/>
         <v>36.3</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="B6" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="B6" s="4" t="s">
-        <v>24</v>
-      </c>
-      <c r="C6" s="4">
-        <v>200.0</v>
-      </c>
-      <c r="D6" s="5">
-        <v>160000.0</v>
-      </c>
       <c r="E6" s="4" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="F6" s="4">
         <v>13.0</v>
@@ -486,26 +450,20 @@
       <c r="K6" s="4">
         <v>25.0</v>
       </c>
-      <c r="L6" s="6">
+      <c r="L6" s="5">
         <f t="shared" si="1"/>
         <v>43.4</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="B7" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="B7" s="4" t="s">
-        <v>26</v>
-      </c>
-      <c r="C7" s="4">
-        <v>198.0</v>
-      </c>
-      <c r="D7" s="5">
-        <v>250000.0</v>
-      </c>
       <c r="E7" s="4" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="F7" s="4">
         <v>7.1</v>
@@ -525,26 +483,20 @@
       <c r="K7" s="4">
         <v>30.0</v>
       </c>
-      <c r="L7" s="6">
+      <c r="L7" s="5">
         <f t="shared" si="1"/>
         <v>36.6</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="B8" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="B8" s="4" t="s">
+      <c r="E8" s="4" t="s">
         <v>28</v>
-      </c>
-      <c r="C8" s="4">
-        <v>187.0</v>
-      </c>
-      <c r="D8" s="5">
-        <v>246000.0</v>
-      </c>
-      <c r="E8" s="4" t="s">
-        <v>29</v>
       </c>
       <c r="F8" s="4">
         <v>6.3</v>
@@ -564,26 +516,20 @@
       <c r="K8" s="4">
         <v>29.0</v>
       </c>
-      <c r="L8" s="6">
+      <c r="L8" s="5">
         <f t="shared" si="1"/>
         <v>34.3</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" s="4" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B9" s="4" t="s">
-        <v>26</v>
-      </c>
-      <c r="C9" s="4">
-        <v>172.0</v>
-      </c>
-      <c r="D9" s="5">
-        <v>210000.0</v>
+        <v>25</v>
       </c>
       <c r="E9" s="4" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="F9" s="4">
         <v>5.0</v>
@@ -603,26 +549,20 @@
       <c r="K9" s="4">
         <v>30.0</v>
       </c>
-      <c r="L9" s="6">
+      <c r="L9" s="5">
         <f t="shared" si="1"/>
         <v>40</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="B10" s="4" t="s">
         <v>31</v>
       </c>
-      <c r="B10" s="4" t="s">
-        <v>32</v>
-      </c>
-      <c r="C10" s="4">
-        <v>189.0</v>
-      </c>
-      <c r="D10" s="5">
-        <v>180200.0</v>
-      </c>
       <c r="E10" s="4" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="F10" s="4">
         <v>8.6</v>
@@ -642,26 +582,20 @@
       <c r="K10" s="4">
         <v>33.0</v>
       </c>
-      <c r="L10" s="6">
+      <c r="L10" s="5">
         <f t="shared" si="1"/>
         <v>37.9</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="B11" s="4" t="s">
         <v>33</v>
       </c>
-      <c r="B11" s="4" t="s">
-        <v>34</v>
-      </c>
-      <c r="C11" s="4">
-        <v>168.0</v>
-      </c>
-      <c r="D11" s="5">
-        <v>145000.0</v>
-      </c>
       <c r="E11" s="4" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="F11" s="4">
         <v>4.6</v>
@@ -681,26 +615,20 @@
       <c r="K11" s="4">
         <v>26.0</v>
       </c>
-      <c r="L11" s="6">
+      <c r="L11" s="5">
         <f t="shared" si="1"/>
         <v>24.4</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" s="4" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B12" s="4" t="s">
-        <v>26</v>
-      </c>
-      <c r="C12" s="4">
-        <v>174.0</v>
-      </c>
-      <c r="D12" s="5">
-        <v>187000.0</v>
+        <v>25</v>
       </c>
       <c r="E12" s="4" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="F12" s="4">
         <v>4.1</v>
@@ -720,26 +648,20 @@
       <c r="K12" s="4">
         <v>28.0</v>
       </c>
-      <c r="L12" s="6">
+      <c r="L12" s="5">
         <f t="shared" si="1"/>
         <v>21.7</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" s="4" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B13" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="C13" s="4">
-        <v>181.0</v>
-      </c>
-      <c r="D13" s="5">
-        <v>196000.0</v>
+        <v>15</v>
       </c>
       <c r="E13" s="4" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="F13" s="4">
         <v>9.5</v>
@@ -759,26 +681,20 @@
       <c r="K13" s="4">
         <v>22.0</v>
       </c>
-      <c r="L13" s="6">
+      <c r="L13" s="5">
         <f t="shared" si="1"/>
         <v>23.3</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="B14" s="4" t="s">
         <v>37</v>
       </c>
-      <c r="B14" s="4" t="s">
-        <v>38</v>
-      </c>
-      <c r="C14" s="4">
-        <v>210.0</v>
-      </c>
-      <c r="D14" s="5">
-        <v>174000.0</v>
-      </c>
       <c r="E14" s="4" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="F14" s="4">
         <v>10.6</v>
@@ -798,26 +714,20 @@
       <c r="K14" s="4">
         <v>22.0</v>
       </c>
-      <c r="L14" s="6">
+      <c r="L14" s="5">
         <f>IFS(E14="Base",SUM(I14,J14,G14),E14="Alero",SUM(H14,J14,F14),E14="Pivot",SUM(F14,J14,I14),E14="Escolta",SUM(H14,J14,G4))</f>
         <v>31.9</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" s="4" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B15" s="4" t="s">
-        <v>26</v>
-      </c>
-      <c r="C15" s="4">
-        <v>184.0</v>
-      </c>
-      <c r="D15" s="5">
-        <v>149000.0</v>
+        <v>25</v>
       </c>
       <c r="E15" s="4" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="F15" s="4">
         <v>7.3</v>
@@ -837,26 +747,20 @@
       <c r="K15" s="4">
         <v>28.0</v>
       </c>
-      <c r="L15" s="6">
+      <c r="L15" s="5">
         <f t="shared" ref="L15:L20" si="2">IFS(E15="Base",SUM(I15,J15,G15),E15="Alero",SUM(H15,J15,F15),E15="Pivot",SUM(F15,J15,I15),E15="Escolta",SUM(H15,J15,G15))</f>
         <v>16.2</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="B16" s="4" t="s">
         <v>40</v>
       </c>
-      <c r="B16" s="4" t="s">
-        <v>41</v>
-      </c>
-      <c r="C16" s="4">
-        <v>178.0</v>
-      </c>
-      <c r="D16" s="5">
-        <v>160000.0</v>
-      </c>
       <c r="E16" s="4" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="F16" s="4">
         <v>5.9</v>
@@ -876,26 +780,20 @@
       <c r="K16" s="4">
         <v>26.0</v>
       </c>
-      <c r="L16" s="6">
+      <c r="L16" s="5">
         <f t="shared" si="2"/>
         <v>25.8</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" s="4" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B17" s="4" t="s">
-        <v>38</v>
-      </c>
-      <c r="C17" s="4">
-        <v>182.0</v>
-      </c>
-      <c r="D17" s="5">
-        <v>150000.0</v>
+        <v>37</v>
       </c>
       <c r="E17" s="4" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="F17" s="4">
         <v>5.0</v>
@@ -915,26 +813,20 @@
       <c r="K17" s="4">
         <v>29.0</v>
       </c>
-      <c r="L17" s="6">
+      <c r="L17" s="5">
         <f t="shared" si="2"/>
         <v>26.6</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" s="4" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B18" s="4" t="s">
-        <v>22</v>
-      </c>
-      <c r="C18" s="4">
-        <v>178.0</v>
-      </c>
-      <c r="D18" s="5">
-        <v>198000.0</v>
+        <v>21</v>
       </c>
       <c r="E18" s="4" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="F18" s="4">
         <v>7.1</v>
@@ -954,26 +846,20 @@
       <c r="K18" s="4">
         <v>28.0</v>
       </c>
-      <c r="L18" s="6">
+      <c r="L18" s="5">
         <f t="shared" si="2"/>
         <v>33.4</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="B19" s="4" t="s">
         <v>44</v>
       </c>
-      <c r="B19" s="4" t="s">
-        <v>45</v>
-      </c>
-      <c r="C19" s="4">
-        <v>198.0</v>
-      </c>
-      <c r="D19" s="5">
-        <v>210000.0</v>
-      </c>
       <c r="E19" s="4" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="F19" s="4">
         <v>10.0</v>
@@ -993,26 +879,20 @@
       <c r="K19" s="4">
         <v>23.0</v>
       </c>
-      <c r="L19" s="6">
+      <c r="L19" s="5">
         <f t="shared" si="2"/>
         <v>36</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" s="4" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B20" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="C20" s="4">
-        <v>166.0</v>
-      </c>
-      <c r="D20" s="5">
-        <v>180000.0</v>
+        <v>27</v>
       </c>
       <c r="E20" s="4" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="F20" s="4">
         <v>5.8</v>
@@ -1032,2950 +912,2950 @@
       <c r="K20" s="4">
         <v>33.0</v>
       </c>
-      <c r="L20" s="6">
+      <c r="L20" s="5">
         <f t="shared" si="2"/>
         <v>29.1</v>
       </c>
     </row>
     <row r="21">
-      <c r="L21" s="7"/>
+      <c r="L21" s="6"/>
     </row>
     <row r="22">
-      <c r="L22" s="7"/>
+      <c r="L22" s="6"/>
     </row>
     <row r="23">
-      <c r="L23" s="7"/>
+      <c r="L23" s="6"/>
     </row>
     <row r="24">
-      <c r="L24" s="7"/>
+      <c r="L24" s="6"/>
     </row>
     <row r="25">
-      <c r="L25" s="7"/>
+      <c r="L25" s="6"/>
     </row>
     <row r="26">
-      <c r="L26" s="7"/>
+      <c r="L26" s="6"/>
     </row>
     <row r="27">
-      <c r="L27" s="7"/>
+      <c r="L27" s="6"/>
     </row>
     <row r="28">
-      <c r="L28" s="7"/>
+      <c r="L28" s="6"/>
     </row>
     <row r="29">
-      <c r="L29" s="7"/>
+      <c r="L29" s="6"/>
     </row>
     <row r="30">
-      <c r="L30" s="7"/>
+      <c r="L30" s="6"/>
     </row>
     <row r="31">
-      <c r="L31" s="7"/>
+      <c r="L31" s="6"/>
     </row>
     <row r="32">
-      <c r="L32" s="7"/>
+      <c r="L32" s="6"/>
     </row>
     <row r="33">
-      <c r="L33" s="7"/>
+      <c r="L33" s="6"/>
     </row>
     <row r="34">
-      <c r="L34" s="7"/>
+      <c r="L34" s="6"/>
     </row>
     <row r="35">
-      <c r="L35" s="7"/>
+      <c r="L35" s="6"/>
     </row>
     <row r="36">
-      <c r="L36" s="7"/>
+      <c r="L36" s="6"/>
     </row>
     <row r="37">
-      <c r="L37" s="7"/>
+      <c r="L37" s="6"/>
     </row>
     <row r="38">
-      <c r="L38" s="7"/>
+      <c r="L38" s="6"/>
     </row>
     <row r="39">
-      <c r="L39" s="7"/>
+      <c r="L39" s="6"/>
     </row>
     <row r="40">
-      <c r="L40" s="7"/>
+      <c r="L40" s="6"/>
     </row>
     <row r="41">
-      <c r="L41" s="7"/>
+      <c r="L41" s="6"/>
     </row>
     <row r="42">
-      <c r="L42" s="7"/>
+      <c r="L42" s="6"/>
     </row>
     <row r="43">
-      <c r="L43" s="7"/>
+      <c r="L43" s="6"/>
     </row>
     <row r="44">
-      <c r="L44" s="7"/>
+      <c r="L44" s="6"/>
     </row>
     <row r="45">
-      <c r="L45" s="7"/>
+      <c r="L45" s="6"/>
     </row>
     <row r="46">
-      <c r="L46" s="7"/>
+      <c r="L46" s="6"/>
     </row>
     <row r="47">
-      <c r="L47" s="7"/>
+      <c r="L47" s="6"/>
     </row>
     <row r="48">
-      <c r="L48" s="7"/>
+      <c r="L48" s="6"/>
     </row>
     <row r="49">
-      <c r="L49" s="7"/>
+      <c r="L49" s="6"/>
     </row>
     <row r="50">
-      <c r="L50" s="7"/>
+      <c r="L50" s="6"/>
     </row>
     <row r="51">
-      <c r="L51" s="7"/>
+      <c r="L51" s="6"/>
     </row>
     <row r="52">
-      <c r="L52" s="7"/>
+      <c r="L52" s="6"/>
     </row>
     <row r="53">
-      <c r="L53" s="7"/>
+      <c r="L53" s="6"/>
     </row>
     <row r="54">
-      <c r="L54" s="7"/>
+      <c r="L54" s="6"/>
     </row>
     <row r="55">
-      <c r="L55" s="7"/>
+      <c r="L55" s="6"/>
     </row>
     <row r="56">
-      <c r="L56" s="7"/>
+      <c r="L56" s="6"/>
     </row>
     <row r="57">
-      <c r="L57" s="7"/>
+      <c r="L57" s="6"/>
     </row>
     <row r="58">
-      <c r="L58" s="7"/>
+      <c r="L58" s="6"/>
     </row>
     <row r="59">
-      <c r="L59" s="7"/>
+      <c r="L59" s="6"/>
     </row>
     <row r="60">
-      <c r="L60" s="7"/>
+      <c r="L60" s="6"/>
     </row>
     <row r="61">
-      <c r="L61" s="7"/>
+      <c r="L61" s="6"/>
     </row>
     <row r="62">
-      <c r="L62" s="7"/>
+      <c r="L62" s="6"/>
     </row>
     <row r="63">
-      <c r="L63" s="7"/>
+      <c r="L63" s="6"/>
     </row>
     <row r="64">
-      <c r="L64" s="7"/>
+      <c r="L64" s="6"/>
     </row>
     <row r="65">
-      <c r="L65" s="7"/>
+      <c r="L65" s="6"/>
     </row>
     <row r="66">
-      <c r="L66" s="7"/>
+      <c r="L66" s="6"/>
     </row>
     <row r="67">
-      <c r="L67" s="7"/>
+      <c r="L67" s="6"/>
     </row>
     <row r="68">
-      <c r="L68" s="7"/>
+      <c r="L68" s="6"/>
     </row>
     <row r="69">
-      <c r="L69" s="7"/>
+      <c r="L69" s="6"/>
     </row>
     <row r="70">
-      <c r="L70" s="7"/>
+      <c r="L70" s="6"/>
     </row>
     <row r="71">
-      <c r="L71" s="7"/>
+      <c r="L71" s="6"/>
     </row>
     <row r="72">
-      <c r="L72" s="7"/>
+      <c r="L72" s="6"/>
     </row>
     <row r="73">
-      <c r="L73" s="7"/>
+      <c r="L73" s="6"/>
     </row>
     <row r="74">
-      <c r="L74" s="7"/>
+      <c r="L74" s="6"/>
     </row>
     <row r="75">
-      <c r="L75" s="7"/>
+      <c r="L75" s="6"/>
     </row>
     <row r="76">
-      <c r="L76" s="7"/>
+      <c r="L76" s="6"/>
     </row>
     <row r="77">
-      <c r="L77" s="7"/>
+      <c r="L77" s="6"/>
     </row>
     <row r="78">
-      <c r="L78" s="7"/>
+      <c r="L78" s="6"/>
     </row>
     <row r="79">
-      <c r="L79" s="7"/>
+      <c r="L79" s="6"/>
     </row>
     <row r="80">
-      <c r="L80" s="7"/>
+      <c r="L80" s="6"/>
     </row>
     <row r="81">
-      <c r="L81" s="7"/>
+      <c r="L81" s="6"/>
     </row>
     <row r="82">
-      <c r="L82" s="7"/>
+      <c r="L82" s="6"/>
     </row>
     <row r="83">
-      <c r="L83" s="7"/>
+      <c r="L83" s="6"/>
     </row>
     <row r="84">
-      <c r="L84" s="7"/>
+      <c r="L84" s="6"/>
     </row>
     <row r="85">
-      <c r="L85" s="7"/>
+      <c r="L85" s="6"/>
     </row>
     <row r="86">
-      <c r="L86" s="7"/>
+      <c r="L86" s="6"/>
     </row>
     <row r="87">
-      <c r="L87" s="7"/>
+      <c r="L87" s="6"/>
     </row>
     <row r="88">
-      <c r="L88" s="7"/>
+      <c r="L88" s="6"/>
     </row>
     <row r="89">
-      <c r="L89" s="7"/>
+      <c r="L89" s="6"/>
     </row>
     <row r="90">
-      <c r="L90" s="7"/>
+      <c r="L90" s="6"/>
     </row>
     <row r="91">
-      <c r="L91" s="7"/>
+      <c r="L91" s="6"/>
     </row>
     <row r="92">
-      <c r="L92" s="7"/>
+      <c r="L92" s="6"/>
     </row>
     <row r="93">
-      <c r="L93" s="7"/>
+      <c r="L93" s="6"/>
     </row>
     <row r="94">
-      <c r="L94" s="7"/>
+      <c r="L94" s="6"/>
     </row>
     <row r="95">
-      <c r="L95" s="7"/>
+      <c r="L95" s="6"/>
     </row>
     <row r="96">
-      <c r="L96" s="7"/>
+      <c r="L96" s="6"/>
     </row>
     <row r="97">
-      <c r="L97" s="7"/>
+      <c r="L97" s="6"/>
     </row>
     <row r="98">
-      <c r="L98" s="7"/>
+      <c r="L98" s="6"/>
     </row>
     <row r="99">
-      <c r="L99" s="7"/>
+      <c r="L99" s="6"/>
     </row>
     <row r="100">
-      <c r="L100" s="7"/>
+      <c r="L100" s="6"/>
     </row>
     <row r="101">
-      <c r="L101" s="7"/>
+      <c r="L101" s="6"/>
     </row>
     <row r="102">
-      <c r="L102" s="7"/>
+      <c r="L102" s="6"/>
     </row>
     <row r="103">
-      <c r="L103" s="7"/>
+      <c r="L103" s="6"/>
     </row>
     <row r="104">
-      <c r="L104" s="7"/>
+      <c r="L104" s="6"/>
     </row>
     <row r="105">
-      <c r="L105" s="7"/>
+      <c r="L105" s="6"/>
     </row>
     <row r="106">
-      <c r="L106" s="7"/>
+      <c r="L106" s="6"/>
     </row>
     <row r="107">
-      <c r="L107" s="7"/>
+      <c r="L107" s="6"/>
     </row>
     <row r="108">
-      <c r="L108" s="7"/>
+      <c r="L108" s="6"/>
     </row>
     <row r="109">
-      <c r="L109" s="7"/>
+      <c r="L109" s="6"/>
     </row>
     <row r="110">
-      <c r="L110" s="7"/>
+      <c r="L110" s="6"/>
     </row>
     <row r="111">
-      <c r="L111" s="7"/>
+      <c r="L111" s="6"/>
     </row>
     <row r="112">
-      <c r="L112" s="7"/>
+      <c r="L112" s="6"/>
     </row>
     <row r="113">
-      <c r="L113" s="7"/>
+      <c r="L113" s="6"/>
     </row>
     <row r="114">
-      <c r="L114" s="7"/>
+      <c r="L114" s="6"/>
     </row>
     <row r="115">
-      <c r="L115" s="7"/>
+      <c r="L115" s="6"/>
     </row>
     <row r="116">
-      <c r="L116" s="7"/>
+      <c r="L116" s="6"/>
     </row>
     <row r="117">
-      <c r="L117" s="7"/>
+      <c r="L117" s="6"/>
     </row>
     <row r="118">
-      <c r="L118" s="7"/>
+      <c r="L118" s="6"/>
     </row>
     <row r="119">
-      <c r="L119" s="7"/>
+      <c r="L119" s="6"/>
     </row>
     <row r="120">
-      <c r="L120" s="7"/>
+      <c r="L120" s="6"/>
     </row>
     <row r="121">
-      <c r="L121" s="7"/>
+      <c r="L121" s="6"/>
     </row>
     <row r="122">
-      <c r="L122" s="7"/>
+      <c r="L122" s="6"/>
     </row>
     <row r="123">
-      <c r="L123" s="7"/>
+      <c r="L123" s="6"/>
     </row>
     <row r="124">
-      <c r="L124" s="7"/>
+      <c r="L124" s="6"/>
     </row>
     <row r="125">
-      <c r="L125" s="7"/>
+      <c r="L125" s="6"/>
     </row>
     <row r="126">
-      <c r="L126" s="7"/>
+      <c r="L126" s="6"/>
     </row>
     <row r="127">
-      <c r="L127" s="7"/>
+      <c r="L127" s="6"/>
     </row>
     <row r="128">
-      <c r="L128" s="7"/>
+      <c r="L128" s="6"/>
     </row>
     <row r="129">
-      <c r="L129" s="7"/>
+      <c r="L129" s="6"/>
     </row>
     <row r="130">
-      <c r="L130" s="7"/>
+      <c r="L130" s="6"/>
     </row>
     <row r="131">
-      <c r="L131" s="7"/>
+      <c r="L131" s="6"/>
     </row>
     <row r="132">
-      <c r="L132" s="7"/>
+      <c r="L132" s="6"/>
     </row>
     <row r="133">
-      <c r="L133" s="7"/>
+      <c r="L133" s="6"/>
     </row>
     <row r="134">
-      <c r="L134" s="7"/>
+      <c r="L134" s="6"/>
     </row>
     <row r="135">
-      <c r="L135" s="7"/>
+      <c r="L135" s="6"/>
     </row>
     <row r="136">
-      <c r="L136" s="7"/>
+      <c r="L136" s="6"/>
     </row>
     <row r="137">
-      <c r="L137" s="7"/>
+      <c r="L137" s="6"/>
     </row>
     <row r="138">
-      <c r="L138" s="7"/>
+      <c r="L138" s="6"/>
     </row>
     <row r="139">
-      <c r="L139" s="7"/>
+      <c r="L139" s="6"/>
     </row>
     <row r="140">
-      <c r="L140" s="7"/>
+      <c r="L140" s="6"/>
     </row>
     <row r="141">
-      <c r="L141" s="7"/>
+      <c r="L141" s="6"/>
     </row>
     <row r="142">
-      <c r="L142" s="7"/>
+      <c r="L142" s="6"/>
     </row>
     <row r="143">
-      <c r="L143" s="7"/>
+      <c r="L143" s="6"/>
     </row>
     <row r="144">
-      <c r="L144" s="7"/>
+      <c r="L144" s="6"/>
     </row>
     <row r="145">
-      <c r="L145" s="7"/>
+      <c r="L145" s="6"/>
     </row>
     <row r="146">
-      <c r="L146" s="7"/>
+      <c r="L146" s="6"/>
     </row>
     <row r="147">
-      <c r="L147" s="7"/>
+      <c r="L147" s="6"/>
     </row>
     <row r="148">
-      <c r="L148" s="7"/>
+      <c r="L148" s="6"/>
     </row>
     <row r="149">
-      <c r="L149" s="7"/>
+      <c r="L149" s="6"/>
     </row>
     <row r="150">
-      <c r="L150" s="7"/>
+      <c r="L150" s="6"/>
     </row>
     <row r="151">
-      <c r="L151" s="7"/>
+      <c r="L151" s="6"/>
     </row>
     <row r="152">
-      <c r="L152" s="7"/>
+      <c r="L152" s="6"/>
     </row>
     <row r="153">
-      <c r="L153" s="7"/>
+      <c r="L153" s="6"/>
     </row>
     <row r="154">
-      <c r="L154" s="7"/>
+      <c r="L154" s="6"/>
     </row>
     <row r="155">
-      <c r="L155" s="7"/>
+      <c r="L155" s="6"/>
     </row>
     <row r="156">
-      <c r="L156" s="7"/>
+      <c r="L156" s="6"/>
     </row>
     <row r="157">
-      <c r="L157" s="7"/>
+      <c r="L157" s="6"/>
     </row>
     <row r="158">
-      <c r="L158" s="7"/>
+      <c r="L158" s="6"/>
     </row>
     <row r="159">
-      <c r="L159" s="7"/>
+      <c r="L159" s="6"/>
     </row>
     <row r="160">
-      <c r="L160" s="7"/>
+      <c r="L160" s="6"/>
     </row>
     <row r="161">
-      <c r="L161" s="7"/>
+      <c r="L161" s="6"/>
     </row>
     <row r="162">
-      <c r="L162" s="7"/>
+      <c r="L162" s="6"/>
     </row>
     <row r="163">
-      <c r="L163" s="7"/>
+      <c r="L163" s="6"/>
     </row>
     <row r="164">
-      <c r="L164" s="7"/>
+      <c r="L164" s="6"/>
     </row>
     <row r="165">
-      <c r="L165" s="7"/>
+      <c r="L165" s="6"/>
     </row>
     <row r="166">
-      <c r="L166" s="7"/>
+      <c r="L166" s="6"/>
     </row>
     <row r="167">
-      <c r="L167" s="7"/>
+      <c r="L167" s="6"/>
     </row>
     <row r="168">
-      <c r="L168" s="7"/>
+      <c r="L168" s="6"/>
     </row>
     <row r="169">
-      <c r="L169" s="7"/>
+      <c r="L169" s="6"/>
     </row>
     <row r="170">
-      <c r="L170" s="7"/>
+      <c r="L170" s="6"/>
     </row>
     <row r="171">
-      <c r="L171" s="7"/>
+      <c r="L171" s="6"/>
     </row>
     <row r="172">
-      <c r="L172" s="7"/>
+      <c r="L172" s="6"/>
     </row>
     <row r="173">
-      <c r="L173" s="7"/>
+      <c r="L173" s="6"/>
     </row>
     <row r="174">
-      <c r="L174" s="7"/>
+      <c r="L174" s="6"/>
     </row>
     <row r="175">
-      <c r="L175" s="7"/>
+      <c r="L175" s="6"/>
     </row>
     <row r="176">
-      <c r="L176" s="7"/>
+      <c r="L176" s="6"/>
     </row>
     <row r="177">
-      <c r="L177" s="7"/>
+      <c r="L177" s="6"/>
     </row>
     <row r="178">
-      <c r="L178" s="7"/>
+      <c r="L178" s="6"/>
     </row>
     <row r="179">
-      <c r="L179" s="7"/>
+      <c r="L179" s="6"/>
     </row>
     <row r="180">
-      <c r="L180" s="7"/>
+      <c r="L180" s="6"/>
     </row>
     <row r="181">
-      <c r="L181" s="7"/>
+      <c r="L181" s="6"/>
     </row>
     <row r="182">
-      <c r="L182" s="7"/>
+      <c r="L182" s="6"/>
     </row>
     <row r="183">
-      <c r="L183" s="7"/>
+      <c r="L183" s="6"/>
     </row>
     <row r="184">
-      <c r="L184" s="7"/>
+      <c r="L184" s="6"/>
     </row>
     <row r="185">
-      <c r="L185" s="7"/>
+      <c r="L185" s="6"/>
     </row>
     <row r="186">
-      <c r="L186" s="7"/>
+      <c r="L186" s="6"/>
     </row>
     <row r="187">
-      <c r="L187" s="7"/>
+      <c r="L187" s="6"/>
     </row>
     <row r="188">
-      <c r="L188" s="7"/>
+      <c r="L188" s="6"/>
     </row>
     <row r="189">
-      <c r="L189" s="7"/>
+      <c r="L189" s="6"/>
     </row>
     <row r="190">
-      <c r="L190" s="7"/>
+      <c r="L190" s="6"/>
     </row>
     <row r="191">
-      <c r="L191" s="7"/>
+      <c r="L191" s="6"/>
     </row>
     <row r="192">
-      <c r="L192" s="7"/>
+      <c r="L192" s="6"/>
     </row>
     <row r="193">
-      <c r="L193" s="7"/>
+      <c r="L193" s="6"/>
     </row>
     <row r="194">
-      <c r="L194" s="7"/>
+      <c r="L194" s="6"/>
     </row>
     <row r="195">
-      <c r="L195" s="7"/>
+      <c r="L195" s="6"/>
     </row>
     <row r="196">
-      <c r="L196" s="7"/>
+      <c r="L196" s="6"/>
     </row>
     <row r="197">
-      <c r="L197" s="7"/>
+      <c r="L197" s="6"/>
     </row>
     <row r="198">
-      <c r="L198" s="7"/>
+      <c r="L198" s="6"/>
     </row>
     <row r="199">
-      <c r="L199" s="7"/>
+      <c r="L199" s="6"/>
     </row>
     <row r="200">
-      <c r="L200" s="7"/>
+      <c r="L200" s="6"/>
     </row>
     <row r="201">
-      <c r="L201" s="7"/>
+      <c r="L201" s="6"/>
     </row>
     <row r="202">
-      <c r="L202" s="7"/>
+      <c r="L202" s="6"/>
     </row>
     <row r="203">
-      <c r="L203" s="7"/>
+      <c r="L203" s="6"/>
     </row>
     <row r="204">
-      <c r="L204" s="7"/>
+      <c r="L204" s="6"/>
     </row>
     <row r="205">
-      <c r="L205" s="7"/>
+      <c r="L205" s="6"/>
     </row>
     <row r="206">
-      <c r="L206" s="7"/>
+      <c r="L206" s="6"/>
     </row>
     <row r="207">
-      <c r="L207" s="7"/>
+      <c r="L207" s="6"/>
     </row>
     <row r="208">
-      <c r="L208" s="7"/>
+      <c r="L208" s="6"/>
     </row>
     <row r="209">
-      <c r="L209" s="7"/>
+      <c r="L209" s="6"/>
     </row>
     <row r="210">
-      <c r="L210" s="7"/>
+      <c r="L210" s="6"/>
     </row>
     <row r="211">
-      <c r="L211" s="7"/>
+      <c r="L211" s="6"/>
     </row>
     <row r="212">
-      <c r="L212" s="7"/>
+      <c r="L212" s="6"/>
     </row>
     <row r="213">
-      <c r="L213" s="7"/>
+      <c r="L213" s="6"/>
     </row>
     <row r="214">
-      <c r="L214" s="7"/>
+      <c r="L214" s="6"/>
     </row>
     <row r="215">
-      <c r="L215" s="7"/>
+      <c r="L215" s="6"/>
     </row>
     <row r="216">
-      <c r="L216" s="7"/>
+      <c r="L216" s="6"/>
     </row>
     <row r="217">
-      <c r="L217" s="7"/>
+      <c r="L217" s="6"/>
     </row>
     <row r="218">
-      <c r="L218" s="7"/>
+      <c r="L218" s="6"/>
     </row>
     <row r="219">
-      <c r="L219" s="7"/>
+      <c r="L219" s="6"/>
     </row>
     <row r="220">
-      <c r="L220" s="7"/>
+      <c r="L220" s="6"/>
     </row>
     <row r="221">
-      <c r="L221" s="7"/>
+      <c r="L221" s="6"/>
     </row>
     <row r="222">
-      <c r="L222" s="7"/>
+      <c r="L222" s="6"/>
     </row>
     <row r="223">
-      <c r="L223" s="7"/>
+      <c r="L223" s="6"/>
     </row>
     <row r="224">
-      <c r="L224" s="7"/>
+      <c r="L224" s="6"/>
     </row>
     <row r="225">
-      <c r="L225" s="7"/>
+      <c r="L225" s="6"/>
     </row>
     <row r="226">
-      <c r="L226" s="7"/>
+      <c r="L226" s="6"/>
     </row>
     <row r="227">
-      <c r="L227" s="7"/>
+      <c r="L227" s="6"/>
     </row>
     <row r="228">
-      <c r="L228" s="7"/>
+      <c r="L228" s="6"/>
     </row>
     <row r="229">
-      <c r="L229" s="7"/>
+      <c r="L229" s="6"/>
     </row>
     <row r="230">
-      <c r="L230" s="7"/>
+      <c r="L230" s="6"/>
     </row>
     <row r="231">
-      <c r="L231" s="7"/>
+      <c r="L231" s="6"/>
     </row>
     <row r="232">
-      <c r="L232" s="7"/>
+      <c r="L232" s="6"/>
     </row>
     <row r="233">
-      <c r="L233" s="7"/>
+      <c r="L233" s="6"/>
     </row>
     <row r="234">
-      <c r="L234" s="7"/>
+      <c r="L234" s="6"/>
     </row>
     <row r="235">
-      <c r="L235" s="7"/>
+      <c r="L235" s="6"/>
     </row>
     <row r="236">
-      <c r="L236" s="7"/>
+      <c r="L236" s="6"/>
     </row>
     <row r="237">
-      <c r="L237" s="7"/>
+      <c r="L237" s="6"/>
     </row>
     <row r="238">
-      <c r="L238" s="7"/>
+      <c r="L238" s="6"/>
     </row>
     <row r="239">
-      <c r="L239" s="7"/>
+      <c r="L239" s="6"/>
     </row>
     <row r="240">
-      <c r="L240" s="7"/>
+      <c r="L240" s="6"/>
     </row>
     <row r="241">
-      <c r="L241" s="7"/>
+      <c r="L241" s="6"/>
     </row>
     <row r="242">
-      <c r="L242" s="7"/>
+      <c r="L242" s="6"/>
     </row>
     <row r="243">
-      <c r="L243" s="7"/>
+      <c r="L243" s="6"/>
     </row>
     <row r="244">
-      <c r="L244" s="7"/>
+      <c r="L244" s="6"/>
     </row>
     <row r="245">
-      <c r="L245" s="7"/>
+      <c r="L245" s="6"/>
     </row>
     <row r="246">
-      <c r="L246" s="7"/>
+      <c r="L246" s="6"/>
     </row>
     <row r="247">
-      <c r="L247" s="7"/>
+      <c r="L247" s="6"/>
     </row>
     <row r="248">
-      <c r="L248" s="7"/>
+      <c r="L248" s="6"/>
     </row>
     <row r="249">
-      <c r="L249" s="7"/>
+      <c r="L249" s="6"/>
     </row>
     <row r="250">
-      <c r="L250" s="7"/>
+      <c r="L250" s="6"/>
     </row>
     <row r="251">
-      <c r="L251" s="7"/>
+      <c r="L251" s="6"/>
     </row>
     <row r="252">
-      <c r="L252" s="7"/>
+      <c r="L252" s="6"/>
     </row>
     <row r="253">
-      <c r="L253" s="7"/>
+      <c r="L253" s="6"/>
     </row>
     <row r="254">
-      <c r="L254" s="7"/>
+      <c r="L254" s="6"/>
     </row>
     <row r="255">
-      <c r="L255" s="7"/>
+      <c r="L255" s="6"/>
     </row>
     <row r="256">
-      <c r="L256" s="7"/>
+      <c r="L256" s="6"/>
     </row>
     <row r="257">
-      <c r="L257" s="7"/>
+      <c r="L257" s="6"/>
     </row>
     <row r="258">
-      <c r="L258" s="7"/>
+      <c r="L258" s="6"/>
     </row>
     <row r="259">
-      <c r="L259" s="7"/>
+      <c r="L259" s="6"/>
     </row>
     <row r="260">
-      <c r="L260" s="7"/>
+      <c r="L260" s="6"/>
     </row>
     <row r="261">
-      <c r="L261" s="7"/>
+      <c r="L261" s="6"/>
     </row>
     <row r="262">
-      <c r="L262" s="7"/>
+      <c r="L262" s="6"/>
     </row>
     <row r="263">
-      <c r="L263" s="7"/>
+      <c r="L263" s="6"/>
     </row>
     <row r="264">
-      <c r="L264" s="7"/>
+      <c r="L264" s="6"/>
     </row>
     <row r="265">
-      <c r="L265" s="7"/>
+      <c r="L265" s="6"/>
     </row>
     <row r="266">
-      <c r="L266" s="7"/>
+      <c r="L266" s="6"/>
     </row>
     <row r="267">
-      <c r="L267" s="7"/>
+      <c r="L267" s="6"/>
     </row>
     <row r="268">
-      <c r="L268" s="7"/>
+      <c r="L268" s="6"/>
     </row>
     <row r="269">
-      <c r="L269" s="7"/>
+      <c r="L269" s="6"/>
     </row>
     <row r="270">
-      <c r="L270" s="7"/>
+      <c r="L270" s="6"/>
     </row>
     <row r="271">
-      <c r="L271" s="7"/>
+      <c r="L271" s="6"/>
     </row>
     <row r="272">
-      <c r="L272" s="7"/>
+      <c r="L272" s="6"/>
     </row>
     <row r="273">
-      <c r="L273" s="7"/>
+      <c r="L273" s="6"/>
     </row>
     <row r="274">
-      <c r="L274" s="7"/>
+      <c r="L274" s="6"/>
     </row>
     <row r="275">
-      <c r="L275" s="7"/>
+      <c r="L275" s="6"/>
     </row>
     <row r="276">
-      <c r="L276" s="7"/>
+      <c r="L276" s="6"/>
     </row>
     <row r="277">
-      <c r="L277" s="7"/>
+      <c r="L277" s="6"/>
     </row>
     <row r="278">
-      <c r="L278" s="7"/>
+      <c r="L278" s="6"/>
     </row>
     <row r="279">
-      <c r="L279" s="7"/>
+      <c r="L279" s="6"/>
     </row>
     <row r="280">
-      <c r="L280" s="7"/>
+      <c r="L280" s="6"/>
     </row>
     <row r="281">
-      <c r="L281" s="7"/>
+      <c r="L281" s="6"/>
     </row>
     <row r="282">
-      <c r="L282" s="7"/>
+      <c r="L282" s="6"/>
     </row>
     <row r="283">
-      <c r="L283" s="7"/>
+      <c r="L283" s="6"/>
     </row>
     <row r="284">
-      <c r="L284" s="7"/>
+      <c r="L284" s="6"/>
     </row>
     <row r="285">
-      <c r="L285" s="7"/>
+      <c r="L285" s="6"/>
     </row>
     <row r="286">
-      <c r="L286" s="7"/>
+      <c r="L286" s="6"/>
     </row>
     <row r="287">
-      <c r="L287" s="7"/>
+      <c r="L287" s="6"/>
     </row>
     <row r="288">
-      <c r="L288" s="7"/>
+      <c r="L288" s="6"/>
     </row>
     <row r="289">
-      <c r="L289" s="7"/>
+      <c r="L289" s="6"/>
     </row>
     <row r="290">
-      <c r="L290" s="7"/>
+      <c r="L290" s="6"/>
     </row>
     <row r="291">
-      <c r="L291" s="7"/>
+      <c r="L291" s="6"/>
     </row>
     <row r="292">
-      <c r="L292" s="7"/>
+      <c r="L292" s="6"/>
     </row>
     <row r="293">
-      <c r="L293" s="7"/>
+      <c r="L293" s="6"/>
     </row>
     <row r="294">
-      <c r="L294" s="7"/>
+      <c r="L294" s="6"/>
     </row>
     <row r="295">
-      <c r="L295" s="7"/>
+      <c r="L295" s="6"/>
     </row>
     <row r="296">
-      <c r="L296" s="7"/>
+      <c r="L296" s="6"/>
     </row>
     <row r="297">
-      <c r="L297" s="7"/>
+      <c r="L297" s="6"/>
     </row>
     <row r="298">
-      <c r="L298" s="7"/>
+      <c r="L298" s="6"/>
     </row>
     <row r="299">
-      <c r="L299" s="7"/>
+      <c r="L299" s="6"/>
     </row>
     <row r="300">
-      <c r="L300" s="7"/>
+      <c r="L300" s="6"/>
     </row>
     <row r="301">
-      <c r="L301" s="7"/>
+      <c r="L301" s="6"/>
     </row>
     <row r="302">
-      <c r="L302" s="7"/>
+      <c r="L302" s="6"/>
     </row>
     <row r="303">
-      <c r="L303" s="7"/>
+      <c r="L303" s="6"/>
     </row>
     <row r="304">
-      <c r="L304" s="7"/>
+      <c r="L304" s="6"/>
     </row>
     <row r="305">
-      <c r="L305" s="7"/>
+      <c r="L305" s="6"/>
     </row>
     <row r="306">
-      <c r="L306" s="7"/>
+      <c r="L306" s="6"/>
     </row>
     <row r="307">
-      <c r="L307" s="7"/>
+      <c r="L307" s="6"/>
     </row>
     <row r="308">
-      <c r="L308" s="7"/>
+      <c r="L308" s="6"/>
     </row>
     <row r="309">
-      <c r="L309" s="7"/>
+      <c r="L309" s="6"/>
     </row>
     <row r="310">
-      <c r="L310" s="7"/>
+      <c r="L310" s="6"/>
     </row>
     <row r="311">
-      <c r="L311" s="7"/>
+      <c r="L311" s="6"/>
     </row>
     <row r="312">
-      <c r="L312" s="7"/>
+      <c r="L312" s="6"/>
     </row>
     <row r="313">
-      <c r="L313" s="7"/>
+      <c r="L313" s="6"/>
     </row>
     <row r="314">
-      <c r="L314" s="7"/>
+      <c r="L314" s="6"/>
     </row>
     <row r="315">
-      <c r="L315" s="7"/>
+      <c r="L315" s="6"/>
     </row>
     <row r="316">
-      <c r="L316" s="7"/>
+      <c r="L316" s="6"/>
     </row>
     <row r="317">
-      <c r="L317" s="7"/>
+      <c r="L317" s="6"/>
     </row>
     <row r="318">
-      <c r="L318" s="7"/>
+      <c r="L318" s="6"/>
     </row>
     <row r="319">
-      <c r="L319" s="7"/>
+      <c r="L319" s="6"/>
     </row>
     <row r="320">
-      <c r="L320" s="7"/>
+      <c r="L320" s="6"/>
     </row>
     <row r="321">
-      <c r="L321" s="7"/>
+      <c r="L321" s="6"/>
     </row>
     <row r="322">
-      <c r="L322" s="7"/>
+      <c r="L322" s="6"/>
     </row>
     <row r="323">
-      <c r="L323" s="7"/>
+      <c r="L323" s="6"/>
     </row>
     <row r="324">
-      <c r="L324" s="7"/>
+      <c r="L324" s="6"/>
     </row>
     <row r="325">
-      <c r="L325" s="7"/>
+      <c r="L325" s="6"/>
     </row>
     <row r="326">
-      <c r="L326" s="7"/>
+      <c r="L326" s="6"/>
     </row>
     <row r="327">
-      <c r="L327" s="7"/>
+      <c r="L327" s="6"/>
     </row>
     <row r="328">
-      <c r="L328" s="7"/>
+      <c r="L328" s="6"/>
     </row>
     <row r="329">
-      <c r="L329" s="7"/>
+      <c r="L329" s="6"/>
     </row>
     <row r="330">
-      <c r="L330" s="7"/>
+      <c r="L330" s="6"/>
     </row>
     <row r="331">
-      <c r="L331" s="7"/>
+      <c r="L331" s="6"/>
     </row>
     <row r="332">
-      <c r="L332" s="7"/>
+      <c r="L332" s="6"/>
     </row>
     <row r="333">
-      <c r="L333" s="7"/>
+      <c r="L333" s="6"/>
     </row>
     <row r="334">
-      <c r="L334" s="7"/>
+      <c r="L334" s="6"/>
     </row>
     <row r="335">
-      <c r="L335" s="7"/>
+      <c r="L335" s="6"/>
     </row>
     <row r="336">
-      <c r="L336" s="7"/>
+      <c r="L336" s="6"/>
     </row>
     <row r="337">
-      <c r="L337" s="7"/>
+      <c r="L337" s="6"/>
     </row>
     <row r="338">
-      <c r="L338" s="7"/>
+      <c r="L338" s="6"/>
     </row>
     <row r="339">
-      <c r="L339" s="7"/>
+      <c r="L339" s="6"/>
     </row>
     <row r="340">
-      <c r="L340" s="7"/>
+      <c r="L340" s="6"/>
     </row>
     <row r="341">
-      <c r="L341" s="7"/>
+      <c r="L341" s="6"/>
     </row>
     <row r="342">
-      <c r="L342" s="7"/>
+      <c r="L342" s="6"/>
     </row>
     <row r="343">
-      <c r="L343" s="7"/>
+      <c r="L343" s="6"/>
     </row>
     <row r="344">
-      <c r="L344" s="7"/>
+      <c r="L344" s="6"/>
     </row>
     <row r="345">
-      <c r="L345" s="7"/>
+      <c r="L345" s="6"/>
     </row>
     <row r="346">
-      <c r="L346" s="7"/>
+      <c r="L346" s="6"/>
     </row>
     <row r="347">
-      <c r="L347" s="7"/>
+      <c r="L347" s="6"/>
     </row>
     <row r="348">
-      <c r="L348" s="7"/>
+      <c r="L348" s="6"/>
     </row>
     <row r="349">
-      <c r="L349" s="7"/>
+      <c r="L349" s="6"/>
     </row>
     <row r="350">
-      <c r="L350" s="7"/>
+      <c r="L350" s="6"/>
     </row>
     <row r="351">
-      <c r="L351" s="7"/>
+      <c r="L351" s="6"/>
     </row>
     <row r="352">
-      <c r="L352" s="7"/>
+      <c r="L352" s="6"/>
     </row>
     <row r="353">
-      <c r="L353" s="7"/>
+      <c r="L353" s="6"/>
     </row>
     <row r="354">
-      <c r="L354" s="7"/>
+      <c r="L354" s="6"/>
     </row>
     <row r="355">
-      <c r="L355" s="7"/>
+      <c r="L355" s="6"/>
     </row>
     <row r="356">
-      <c r="L356" s="7"/>
+      <c r="L356" s="6"/>
     </row>
     <row r="357">
-      <c r="L357" s="7"/>
+      <c r="L357" s="6"/>
     </row>
     <row r="358">
-      <c r="L358" s="7"/>
+      <c r="L358" s="6"/>
     </row>
     <row r="359">
-      <c r="L359" s="7"/>
+      <c r="L359" s="6"/>
     </row>
     <row r="360">
-      <c r="L360" s="7"/>
+      <c r="L360" s="6"/>
     </row>
     <row r="361">
-      <c r="L361" s="7"/>
+      <c r="L361" s="6"/>
     </row>
     <row r="362">
-      <c r="L362" s="7"/>
+      <c r="L362" s="6"/>
     </row>
     <row r="363">
-      <c r="L363" s="7"/>
+      <c r="L363" s="6"/>
     </row>
     <row r="364">
-      <c r="L364" s="7"/>
+      <c r="L364" s="6"/>
     </row>
     <row r="365">
-      <c r="L365" s="7"/>
+      <c r="L365" s="6"/>
     </row>
     <row r="366">
-      <c r="L366" s="7"/>
+      <c r="L366" s="6"/>
     </row>
     <row r="367">
-      <c r="L367" s="7"/>
+      <c r="L367" s="6"/>
     </row>
     <row r="368">
-      <c r="L368" s="7"/>
+      <c r="L368" s="6"/>
     </row>
     <row r="369">
-      <c r="L369" s="7"/>
+      <c r="L369" s="6"/>
     </row>
     <row r="370">
-      <c r="L370" s="7"/>
+      <c r="L370" s="6"/>
     </row>
     <row r="371">
-      <c r="L371" s="7"/>
+      <c r="L371" s="6"/>
     </row>
     <row r="372">
-      <c r="L372" s="7"/>
+      <c r="L372" s="6"/>
     </row>
     <row r="373">
-      <c r="L373" s="7"/>
+      <c r="L373" s="6"/>
     </row>
     <row r="374">
-      <c r="L374" s="7"/>
+      <c r="L374" s="6"/>
     </row>
     <row r="375">
-      <c r="L375" s="7"/>
+      <c r="L375" s="6"/>
     </row>
     <row r="376">
-      <c r="L376" s="7"/>
+      <c r="L376" s="6"/>
     </row>
     <row r="377">
-      <c r="L377" s="7"/>
+      <c r="L377" s="6"/>
     </row>
     <row r="378">
-      <c r="L378" s="7"/>
+      <c r="L378" s="6"/>
     </row>
     <row r="379">
-      <c r="L379" s="7"/>
+      <c r="L379" s="6"/>
     </row>
     <row r="380">
-      <c r="L380" s="7"/>
+      <c r="L380" s="6"/>
     </row>
     <row r="381">
-      <c r="L381" s="7"/>
+      <c r="L381" s="6"/>
     </row>
     <row r="382">
-      <c r="L382" s="7"/>
+      <c r="L382" s="6"/>
     </row>
     <row r="383">
-      <c r="L383" s="7"/>
+      <c r="L383" s="6"/>
     </row>
     <row r="384">
-      <c r="L384" s="7"/>
+      <c r="L384" s="6"/>
     </row>
     <row r="385">
-      <c r="L385" s="7"/>
+      <c r="L385" s="6"/>
     </row>
     <row r="386">
-      <c r="L386" s="7"/>
+      <c r="L386" s="6"/>
     </row>
     <row r="387">
-      <c r="L387" s="7"/>
+      <c r="L387" s="6"/>
     </row>
     <row r="388">
-      <c r="L388" s="7"/>
+      <c r="L388" s="6"/>
     </row>
     <row r="389">
-      <c r="L389" s="7"/>
+      <c r="L389" s="6"/>
     </row>
     <row r="390">
-      <c r="L390" s="7"/>
+      <c r="L390" s="6"/>
     </row>
     <row r="391">
-      <c r="L391" s="7"/>
+      <c r="L391" s="6"/>
     </row>
     <row r="392">
-      <c r="L392" s="7"/>
+      <c r="L392" s="6"/>
     </row>
     <row r="393">
-      <c r="L393" s="7"/>
+      <c r="L393" s="6"/>
     </row>
     <row r="394">
-      <c r="L394" s="7"/>
+      <c r="L394" s="6"/>
     </row>
     <row r="395">
-      <c r="L395" s="7"/>
+      <c r="L395" s="6"/>
     </row>
     <row r="396">
-      <c r="L396" s="7"/>
+      <c r="L396" s="6"/>
     </row>
     <row r="397">
-      <c r="L397" s="7"/>
+      <c r="L397" s="6"/>
     </row>
     <row r="398">
-      <c r="L398" s="7"/>
+      <c r="L398" s="6"/>
     </row>
     <row r="399">
-      <c r="L399" s="7"/>
+      <c r="L399" s="6"/>
     </row>
     <row r="400">
-      <c r="L400" s="7"/>
+      <c r="L400" s="6"/>
     </row>
     <row r="401">
-      <c r="L401" s="7"/>
+      <c r="L401" s="6"/>
     </row>
     <row r="402">
-      <c r="L402" s="7"/>
+      <c r="L402" s="6"/>
     </row>
     <row r="403">
-      <c r="L403" s="7"/>
+      <c r="L403" s="6"/>
     </row>
     <row r="404">
-      <c r="L404" s="7"/>
+      <c r="L404" s="6"/>
     </row>
     <row r="405">
-      <c r="L405" s="7"/>
+      <c r="L405" s="6"/>
     </row>
     <row r="406">
-      <c r="L406" s="7"/>
+      <c r="L406" s="6"/>
     </row>
     <row r="407">
-      <c r="L407" s="7"/>
+      <c r="L407" s="6"/>
     </row>
     <row r="408">
-      <c r="L408" s="7"/>
+      <c r="L408" s="6"/>
     </row>
     <row r="409">
-      <c r="L409" s="7"/>
+      <c r="L409" s="6"/>
     </row>
     <row r="410">
-      <c r="L410" s="7"/>
+      <c r="L410" s="6"/>
     </row>
     <row r="411">
-      <c r="L411" s="7"/>
+      <c r="L411" s="6"/>
     </row>
     <row r="412">
-      <c r="L412" s="7"/>
+      <c r="L412" s="6"/>
     </row>
     <row r="413">
-      <c r="L413" s="7"/>
+      <c r="L413" s="6"/>
     </row>
     <row r="414">
-      <c r="L414" s="7"/>
+      <c r="L414" s="6"/>
     </row>
     <row r="415">
-      <c r="L415" s="7"/>
+      <c r="L415" s="6"/>
     </row>
     <row r="416">
-      <c r="L416" s="7"/>
+      <c r="L416" s="6"/>
     </row>
     <row r="417">
-      <c r="L417" s="7"/>
+      <c r="L417" s="6"/>
     </row>
     <row r="418">
-      <c r="L418" s="7"/>
+      <c r="L418" s="6"/>
     </row>
     <row r="419">
-      <c r="L419" s="7"/>
+      <c r="L419" s="6"/>
     </row>
     <row r="420">
-      <c r="L420" s="7"/>
+      <c r="L420" s="6"/>
     </row>
     <row r="421">
-      <c r="L421" s="7"/>
+      <c r="L421" s="6"/>
     </row>
     <row r="422">
-      <c r="L422" s="7"/>
+      <c r="L422" s="6"/>
     </row>
     <row r="423">
-      <c r="L423" s="7"/>
+      <c r="L423" s="6"/>
     </row>
     <row r="424">
-      <c r="L424" s="7"/>
+      <c r="L424" s="6"/>
     </row>
     <row r="425">
-      <c r="L425" s="7"/>
+      <c r="L425" s="6"/>
     </row>
     <row r="426">
-      <c r="L426" s="7"/>
+      <c r="L426" s="6"/>
     </row>
     <row r="427">
-      <c r="L427" s="7"/>
+      <c r="L427" s="6"/>
     </row>
     <row r="428">
-      <c r="L428" s="7"/>
+      <c r="L428" s="6"/>
     </row>
     <row r="429">
-      <c r="L429" s="7"/>
+      <c r="L429" s="6"/>
     </row>
     <row r="430">
-      <c r="L430" s="7"/>
+      <c r="L430" s="6"/>
     </row>
     <row r="431">
-      <c r="L431" s="7"/>
+      <c r="L431" s="6"/>
     </row>
     <row r="432">
-      <c r="L432" s="7"/>
+      <c r="L432" s="6"/>
     </row>
     <row r="433">
-      <c r="L433" s="7"/>
+      <c r="L433" s="6"/>
     </row>
     <row r="434">
-      <c r="L434" s="7"/>
+      <c r="L434" s="6"/>
     </row>
     <row r="435">
-      <c r="L435" s="7"/>
+      <c r="L435" s="6"/>
     </row>
     <row r="436">
-      <c r="L436" s="7"/>
+      <c r="L436" s="6"/>
     </row>
     <row r="437">
-      <c r="L437" s="7"/>
+      <c r="L437" s="6"/>
     </row>
     <row r="438">
-      <c r="L438" s="7"/>
+      <c r="L438" s="6"/>
     </row>
     <row r="439">
-      <c r="L439" s="7"/>
+      <c r="L439" s="6"/>
     </row>
     <row r="440">
-      <c r="L440" s="7"/>
+      <c r="L440" s="6"/>
     </row>
     <row r="441">
-      <c r="L441" s="7"/>
+      <c r="L441" s="6"/>
     </row>
     <row r="442">
-      <c r="L442" s="7"/>
+      <c r="L442" s="6"/>
     </row>
     <row r="443">
-      <c r="L443" s="7"/>
+      <c r="L443" s="6"/>
     </row>
     <row r="444">
-      <c r="L444" s="7"/>
+      <c r="L444" s="6"/>
     </row>
     <row r="445">
-      <c r="L445" s="7"/>
+      <c r="L445" s="6"/>
     </row>
     <row r="446">
-      <c r="L446" s="7"/>
+      <c r="L446" s="6"/>
     </row>
     <row r="447">
-      <c r="L447" s="7"/>
+      <c r="L447" s="6"/>
     </row>
     <row r="448">
-      <c r="L448" s="7"/>
+      <c r="L448" s="6"/>
     </row>
     <row r="449">
-      <c r="L449" s="7"/>
+      <c r="L449" s="6"/>
     </row>
     <row r="450">
-      <c r="L450" s="7"/>
+      <c r="L450" s="6"/>
     </row>
     <row r="451">
-      <c r="L451" s="7"/>
+      <c r="L451" s="6"/>
     </row>
     <row r="452">
-      <c r="L452" s="7"/>
+      <c r="L452" s="6"/>
     </row>
     <row r="453">
-      <c r="L453" s="7"/>
+      <c r="L453" s="6"/>
     </row>
     <row r="454">
-      <c r="L454" s="7"/>
+      <c r="L454" s="6"/>
     </row>
     <row r="455">
-      <c r="L455" s="7"/>
+      <c r="L455" s="6"/>
     </row>
     <row r="456">
-      <c r="L456" s="7"/>
+      <c r="L456" s="6"/>
     </row>
     <row r="457">
-      <c r="L457" s="7"/>
+      <c r="L457" s="6"/>
     </row>
     <row r="458">
-      <c r="L458" s="7"/>
+      <c r="L458" s="6"/>
     </row>
     <row r="459">
-      <c r="L459" s="7"/>
+      <c r="L459" s="6"/>
     </row>
     <row r="460">
-      <c r="L460" s="7"/>
+      <c r="L460" s="6"/>
     </row>
     <row r="461">
-      <c r="L461" s="7"/>
+      <c r="L461" s="6"/>
     </row>
     <row r="462">
-      <c r="L462" s="7"/>
+      <c r="L462" s="6"/>
     </row>
     <row r="463">
-      <c r="L463" s="7"/>
+      <c r="L463" s="6"/>
     </row>
     <row r="464">
-      <c r="L464" s="7"/>
+      <c r="L464" s="6"/>
     </row>
     <row r="465">
-      <c r="L465" s="7"/>
+      <c r="L465" s="6"/>
     </row>
     <row r="466">
-      <c r="L466" s="7"/>
+      <c r="L466" s="6"/>
     </row>
     <row r="467">
-      <c r="L467" s="7"/>
+      <c r="L467" s="6"/>
     </row>
     <row r="468">
-      <c r="L468" s="7"/>
+      <c r="L468" s="6"/>
     </row>
     <row r="469">
-      <c r="L469" s="7"/>
+      <c r="L469" s="6"/>
     </row>
     <row r="470">
-      <c r="L470" s="7"/>
+      <c r="L470" s="6"/>
     </row>
     <row r="471">
-      <c r="L471" s="7"/>
+      <c r="L471" s="6"/>
     </row>
     <row r="472">
-      <c r="L472" s="7"/>
+      <c r="L472" s="6"/>
     </row>
     <row r="473">
-      <c r="L473" s="7"/>
+      <c r="L473" s="6"/>
     </row>
     <row r="474">
-      <c r="L474" s="7"/>
+      <c r="L474" s="6"/>
     </row>
     <row r="475">
-      <c r="L475" s="7"/>
+      <c r="L475" s="6"/>
     </row>
     <row r="476">
-      <c r="L476" s="7"/>
+      <c r="L476" s="6"/>
     </row>
     <row r="477">
-      <c r="L477" s="7"/>
+      <c r="L477" s="6"/>
     </row>
     <row r="478">
-      <c r="L478" s="7"/>
+      <c r="L478" s="6"/>
     </row>
     <row r="479">
-      <c r="L479" s="7"/>
+      <c r="L479" s="6"/>
     </row>
     <row r="480">
-      <c r="L480" s="7"/>
+      <c r="L480" s="6"/>
     </row>
     <row r="481">
-      <c r="L481" s="7"/>
+      <c r="L481" s="6"/>
     </row>
     <row r="482">
-      <c r="L482" s="7"/>
+      <c r="L482" s="6"/>
     </row>
     <row r="483">
-      <c r="L483" s="7"/>
+      <c r="L483" s="6"/>
     </row>
     <row r="484">
-      <c r="L484" s="7"/>
+      <c r="L484" s="6"/>
     </row>
     <row r="485">
-      <c r="L485" s="7"/>
+      <c r="L485" s="6"/>
     </row>
     <row r="486">
-      <c r="L486" s="7"/>
+      <c r="L486" s="6"/>
     </row>
     <row r="487">
-      <c r="L487" s="7"/>
+      <c r="L487" s="6"/>
     </row>
     <row r="488">
-      <c r="L488" s="7"/>
+      <c r="L488" s="6"/>
     </row>
     <row r="489">
-      <c r="L489" s="7"/>
+      <c r="L489" s="6"/>
     </row>
     <row r="490">
-      <c r="L490" s="7"/>
+      <c r="L490" s="6"/>
     </row>
     <row r="491">
-      <c r="L491" s="7"/>
+      <c r="L491" s="6"/>
     </row>
     <row r="492">
-      <c r="L492" s="7"/>
+      <c r="L492" s="6"/>
     </row>
     <row r="493">
-      <c r="L493" s="7"/>
+      <c r="L493" s="6"/>
     </row>
     <row r="494">
-      <c r="L494" s="7"/>
+      <c r="L494" s="6"/>
     </row>
     <row r="495">
-      <c r="L495" s="7"/>
+      <c r="L495" s="6"/>
     </row>
     <row r="496">
-      <c r="L496" s="7"/>
+      <c r="L496" s="6"/>
     </row>
     <row r="497">
-      <c r="L497" s="7"/>
+      <c r="L497" s="6"/>
     </row>
     <row r="498">
-      <c r="L498" s="7"/>
+      <c r="L498" s="6"/>
     </row>
     <row r="499">
-      <c r="L499" s="7"/>
+      <c r="L499" s="6"/>
     </row>
     <row r="500">
-      <c r="L500" s="7"/>
+      <c r="L500" s="6"/>
     </row>
     <row r="501">
-      <c r="L501" s="7"/>
+      <c r="L501" s="6"/>
     </row>
     <row r="502">
-      <c r="L502" s="7"/>
+      <c r="L502" s="6"/>
     </row>
     <row r="503">
-      <c r="L503" s="7"/>
+      <c r="L503" s="6"/>
     </row>
     <row r="504">
-      <c r="L504" s="7"/>
+      <c r="L504" s="6"/>
     </row>
     <row r="505">
-      <c r="L505" s="7"/>
+      <c r="L505" s="6"/>
     </row>
     <row r="506">
-      <c r="L506" s="7"/>
+      <c r="L506" s="6"/>
     </row>
     <row r="507">
-      <c r="L507" s="7"/>
+      <c r="L507" s="6"/>
     </row>
     <row r="508">
-      <c r="L508" s="7"/>
+      <c r="L508" s="6"/>
     </row>
     <row r="509">
-      <c r="L509" s="7"/>
+      <c r="L509" s="6"/>
     </row>
     <row r="510">
-      <c r="L510" s="7"/>
+      <c r="L510" s="6"/>
     </row>
     <row r="511">
-      <c r="L511" s="7"/>
+      <c r="L511" s="6"/>
     </row>
     <row r="512">
-      <c r="L512" s="7"/>
+      <c r="L512" s="6"/>
     </row>
     <row r="513">
-      <c r="L513" s="7"/>
+      <c r="L513" s="6"/>
     </row>
     <row r="514">
-      <c r="L514" s="7"/>
+      <c r="L514" s="6"/>
     </row>
     <row r="515">
-      <c r="L515" s="7"/>
+      <c r="L515" s="6"/>
     </row>
     <row r="516">
-      <c r="L516" s="7"/>
+      <c r="L516" s="6"/>
     </row>
     <row r="517">
-      <c r="L517" s="7"/>
+      <c r="L517" s="6"/>
     </row>
     <row r="518">
-      <c r="L518" s="7"/>
+      <c r="L518" s="6"/>
     </row>
     <row r="519">
-      <c r="L519" s="7"/>
+      <c r="L519" s="6"/>
     </row>
     <row r="520">
-      <c r="L520" s="7"/>
+      <c r="L520" s="6"/>
     </row>
     <row r="521">
-      <c r="L521" s="7"/>
+      <c r="L521" s="6"/>
     </row>
     <row r="522">
-      <c r="L522" s="7"/>
+      <c r="L522" s="6"/>
     </row>
     <row r="523">
-      <c r="L523" s="7"/>
+      <c r="L523" s="6"/>
     </row>
     <row r="524">
-      <c r="L524" s="7"/>
+      <c r="L524" s="6"/>
     </row>
     <row r="525">
-      <c r="L525" s="7"/>
+      <c r="L525" s="6"/>
     </row>
     <row r="526">
-      <c r="L526" s="7"/>
+      <c r="L526" s="6"/>
     </row>
     <row r="527">
-      <c r="L527" s="7"/>
+      <c r="L527" s="6"/>
     </row>
     <row r="528">
-      <c r="L528" s="7"/>
+      <c r="L528" s="6"/>
     </row>
     <row r="529">
-      <c r="L529" s="7"/>
+      <c r="L529" s="6"/>
     </row>
     <row r="530">
-      <c r="L530" s="7"/>
+      <c r="L530" s="6"/>
     </row>
     <row r="531">
-      <c r="L531" s="7"/>
+      <c r="L531" s="6"/>
     </row>
     <row r="532">
-      <c r="L532" s="7"/>
+      <c r="L532" s="6"/>
     </row>
     <row r="533">
-      <c r="L533" s="7"/>
+      <c r="L533" s="6"/>
     </row>
     <row r="534">
-      <c r="L534" s="7"/>
+      <c r="L534" s="6"/>
     </row>
     <row r="535">
-      <c r="L535" s="7"/>
+      <c r="L535" s="6"/>
     </row>
     <row r="536">
-      <c r="L536" s="7"/>
+      <c r="L536" s="6"/>
     </row>
     <row r="537">
-      <c r="L537" s="7"/>
+      <c r="L537" s="6"/>
     </row>
     <row r="538">
-      <c r="L538" s="7"/>
+      <c r="L538" s="6"/>
     </row>
     <row r="539">
-      <c r="L539" s="7"/>
+      <c r="L539" s="6"/>
     </row>
     <row r="540">
-      <c r="L540" s="7"/>
+      <c r="L540" s="6"/>
     </row>
     <row r="541">
-      <c r="L541" s="7"/>
+      <c r="L541" s="6"/>
     </row>
     <row r="542">
-      <c r="L542" s="7"/>
+      <c r="L542" s="6"/>
     </row>
     <row r="543">
-      <c r="L543" s="7"/>
+      <c r="L543" s="6"/>
     </row>
     <row r="544">
-      <c r="L544" s="7"/>
+      <c r="L544" s="6"/>
     </row>
     <row r="545">
-      <c r="L545" s="7"/>
+      <c r="L545" s="6"/>
     </row>
     <row r="546">
-      <c r="L546" s="7"/>
+      <c r="L546" s="6"/>
     </row>
     <row r="547">
-      <c r="L547" s="7"/>
+      <c r="L547" s="6"/>
     </row>
     <row r="548">
-      <c r="L548" s="7"/>
+      <c r="L548" s="6"/>
     </row>
     <row r="549">
-      <c r="L549" s="7"/>
+      <c r="L549" s="6"/>
     </row>
     <row r="550">
-      <c r="L550" s="7"/>
+      <c r="L550" s="6"/>
     </row>
     <row r="551">
-      <c r="L551" s="7"/>
+      <c r="L551" s="6"/>
     </row>
     <row r="552">
-      <c r="L552" s="7"/>
+      <c r="L552" s="6"/>
     </row>
     <row r="553">
-      <c r="L553" s="7"/>
+      <c r="L553" s="6"/>
     </row>
     <row r="554">
-      <c r="L554" s="7"/>
+      <c r="L554" s="6"/>
     </row>
     <row r="555">
-      <c r="L555" s="7"/>
+      <c r="L555" s="6"/>
     </row>
     <row r="556">
-      <c r="L556" s="7"/>
+      <c r="L556" s="6"/>
     </row>
     <row r="557">
-      <c r="L557" s="7"/>
+      <c r="L557" s="6"/>
     </row>
     <row r="558">
-      <c r="L558" s="7"/>
+      <c r="L558" s="6"/>
     </row>
     <row r="559">
-      <c r="L559" s="7"/>
+      <c r="L559" s="6"/>
     </row>
     <row r="560">
-      <c r="L560" s="7"/>
+      <c r="L560" s="6"/>
     </row>
     <row r="561">
-      <c r="L561" s="7"/>
+      <c r="L561" s="6"/>
     </row>
     <row r="562">
-      <c r="L562" s="7"/>
+      <c r="L562" s="6"/>
     </row>
     <row r="563">
-      <c r="L563" s="7"/>
+      <c r="L563" s="6"/>
     </row>
     <row r="564">
-      <c r="L564" s="7"/>
+      <c r="L564" s="6"/>
     </row>
     <row r="565">
-      <c r="L565" s="7"/>
+      <c r="L565" s="6"/>
     </row>
     <row r="566">
-      <c r="L566" s="7"/>
+      <c r="L566" s="6"/>
     </row>
     <row r="567">
-      <c r="L567" s="7"/>
+      <c r="L567" s="6"/>
     </row>
     <row r="568">
-      <c r="L568" s="7"/>
+      <c r="L568" s="6"/>
     </row>
     <row r="569">
-      <c r="L569" s="7"/>
+      <c r="L569" s="6"/>
     </row>
     <row r="570">
-      <c r="L570" s="7"/>
+      <c r="L570" s="6"/>
     </row>
     <row r="571">
-      <c r="L571" s="7"/>
+      <c r="L571" s="6"/>
     </row>
     <row r="572">
-      <c r="L572" s="7"/>
+      <c r="L572" s="6"/>
     </row>
     <row r="573">
-      <c r="L573" s="7"/>
+      <c r="L573" s="6"/>
     </row>
     <row r="574">
-      <c r="L574" s="7"/>
+      <c r="L574" s="6"/>
     </row>
     <row r="575">
-      <c r="L575" s="7"/>
+      <c r="L575" s="6"/>
     </row>
     <row r="576">
-      <c r="L576" s="7"/>
+      <c r="L576" s="6"/>
     </row>
     <row r="577">
-      <c r="L577" s="7"/>
+      <c r="L577" s="6"/>
     </row>
     <row r="578">
-      <c r="L578" s="7"/>
+      <c r="L578" s="6"/>
     </row>
     <row r="579">
-      <c r="L579" s="7"/>
+      <c r="L579" s="6"/>
     </row>
     <row r="580">
-      <c r="L580" s="7"/>
+      <c r="L580" s="6"/>
     </row>
     <row r="581">
-      <c r="L581" s="7"/>
+      <c r="L581" s="6"/>
     </row>
     <row r="582">
-      <c r="L582" s="7"/>
+      <c r="L582" s="6"/>
     </row>
     <row r="583">
-      <c r="L583" s="7"/>
+      <c r="L583" s="6"/>
     </row>
     <row r="584">
-      <c r="L584" s="7"/>
+      <c r="L584" s="6"/>
     </row>
     <row r="585">
-      <c r="L585" s="7"/>
+      <c r="L585" s="6"/>
     </row>
     <row r="586">
-      <c r="L586" s="7"/>
+      <c r="L586" s="6"/>
     </row>
     <row r="587">
-      <c r="L587" s="7"/>
+      <c r="L587" s="6"/>
     </row>
     <row r="588">
-      <c r="L588" s="7"/>
+      <c r="L588" s="6"/>
     </row>
     <row r="589">
-      <c r="L589" s="7"/>
+      <c r="L589" s="6"/>
     </row>
     <row r="590">
-      <c r="L590" s="7"/>
+      <c r="L590" s="6"/>
     </row>
     <row r="591">
-      <c r="L591" s="7"/>
+      <c r="L591" s="6"/>
     </row>
     <row r="592">
-      <c r="L592" s="7"/>
+      <c r="L592" s="6"/>
     </row>
     <row r="593">
-      <c r="L593" s="7"/>
+      <c r="L593" s="6"/>
     </row>
     <row r="594">
-      <c r="L594" s="7"/>
+      <c r="L594" s="6"/>
     </row>
     <row r="595">
-      <c r="L595" s="7"/>
+      <c r="L595" s="6"/>
     </row>
     <row r="596">
-      <c r="L596" s="7"/>
+      <c r="L596" s="6"/>
     </row>
     <row r="597">
-      <c r="L597" s="7"/>
+      <c r="L597" s="6"/>
     </row>
     <row r="598">
-      <c r="L598" s="7"/>
+      <c r="L598" s="6"/>
     </row>
     <row r="599">
-      <c r="L599" s="7"/>
+      <c r="L599" s="6"/>
     </row>
     <row r="600">
-      <c r="L600" s="7"/>
+      <c r="L600" s="6"/>
     </row>
     <row r="601">
-      <c r="L601" s="7"/>
+      <c r="L601" s="6"/>
     </row>
     <row r="602">
-      <c r="L602" s="7"/>
+      <c r="L602" s="6"/>
     </row>
     <row r="603">
-      <c r="L603" s="7"/>
+      <c r="L603" s="6"/>
     </row>
     <row r="604">
-      <c r="L604" s="7"/>
+      <c r="L604" s="6"/>
     </row>
     <row r="605">
-      <c r="L605" s="7"/>
+      <c r="L605" s="6"/>
     </row>
     <row r="606">
-      <c r="L606" s="7"/>
+      <c r="L606" s="6"/>
     </row>
     <row r="607">
-      <c r="L607" s="7"/>
+      <c r="L607" s="6"/>
     </row>
     <row r="608">
-      <c r="L608" s="7"/>
+      <c r="L608" s="6"/>
     </row>
     <row r="609">
-      <c r="L609" s="7"/>
+      <c r="L609" s="6"/>
     </row>
     <row r="610">
-      <c r="L610" s="7"/>
+      <c r="L610" s="6"/>
     </row>
     <row r="611">
-      <c r="L611" s="7"/>
+      <c r="L611" s="6"/>
     </row>
     <row r="612">
-      <c r="L612" s="7"/>
+      <c r="L612" s="6"/>
     </row>
     <row r="613">
-      <c r="L613" s="7"/>
+      <c r="L613" s="6"/>
     </row>
     <row r="614">
-      <c r="L614" s="7"/>
+      <c r="L614" s="6"/>
     </row>
     <row r="615">
-      <c r="L615" s="7"/>
+      <c r="L615" s="6"/>
     </row>
     <row r="616">
-      <c r="L616" s="7"/>
+      <c r="L616" s="6"/>
     </row>
     <row r="617">
-      <c r="L617" s="7"/>
+      <c r="L617" s="6"/>
     </row>
     <row r="618">
-      <c r="L618" s="7"/>
+      <c r="L618" s="6"/>
     </row>
     <row r="619">
-      <c r="L619" s="7"/>
+      <c r="L619" s="6"/>
     </row>
     <row r="620">
-      <c r="L620" s="7"/>
+      <c r="L620" s="6"/>
     </row>
     <row r="621">
-      <c r="L621" s="7"/>
+      <c r="L621" s="6"/>
     </row>
     <row r="622">
-      <c r="L622" s="7"/>
+      <c r="L622" s="6"/>
     </row>
     <row r="623">
-      <c r="L623" s="7"/>
+      <c r="L623" s="6"/>
     </row>
     <row r="624">
-      <c r="L624" s="7"/>
+      <c r="L624" s="6"/>
     </row>
     <row r="625">
-      <c r="L625" s="7"/>
+      <c r="L625" s="6"/>
     </row>
     <row r="626">
-      <c r="L626" s="7"/>
+      <c r="L626" s="6"/>
     </row>
     <row r="627">
-      <c r="L627" s="7"/>
+      <c r="L627" s="6"/>
     </row>
     <row r="628">
-      <c r="L628" s="7"/>
+      <c r="L628" s="6"/>
     </row>
     <row r="629">
-      <c r="L629" s="7"/>
+      <c r="L629" s="6"/>
     </row>
     <row r="630">
-      <c r="L630" s="7"/>
+      <c r="L630" s="6"/>
     </row>
     <row r="631">
-      <c r="L631" s="7"/>
+      <c r="L631" s="6"/>
     </row>
     <row r="632">
-      <c r="L632" s="7"/>
+      <c r="L632" s="6"/>
     </row>
     <row r="633">
-      <c r="L633" s="7"/>
+      <c r="L633" s="6"/>
     </row>
     <row r="634">
-      <c r="L634" s="7"/>
+      <c r="L634" s="6"/>
     </row>
     <row r="635">
-      <c r="L635" s="7"/>
+      <c r="L635" s="6"/>
     </row>
     <row r="636">
-      <c r="L636" s="7"/>
+      <c r="L636" s="6"/>
     </row>
     <row r="637">
-      <c r="L637" s="7"/>
+      <c r="L637" s="6"/>
     </row>
     <row r="638">
-      <c r="L638" s="7"/>
+      <c r="L638" s="6"/>
     </row>
     <row r="639">
-      <c r="L639" s="7"/>
+      <c r="L639" s="6"/>
     </row>
     <row r="640">
-      <c r="L640" s="7"/>
+      <c r="L640" s="6"/>
     </row>
     <row r="641">
-      <c r="L641" s="7"/>
+      <c r="L641" s="6"/>
     </row>
     <row r="642">
-      <c r="L642" s="7"/>
+      <c r="L642" s="6"/>
     </row>
     <row r="643">
-      <c r="L643" s="7"/>
+      <c r="L643" s="6"/>
     </row>
     <row r="644">
-      <c r="L644" s="7"/>
+      <c r="L644" s="6"/>
     </row>
     <row r="645">
-      <c r="L645" s="7"/>
+      <c r="L645" s="6"/>
     </row>
     <row r="646">
-      <c r="L646" s="7"/>
+      <c r="L646" s="6"/>
     </row>
     <row r="647">
-      <c r="L647" s="7"/>
+      <c r="L647" s="6"/>
     </row>
     <row r="648">
-      <c r="L648" s="7"/>
+      <c r="L648" s="6"/>
     </row>
     <row r="649">
-      <c r="L649" s="7"/>
+      <c r="L649" s="6"/>
     </row>
     <row r="650">
-      <c r="L650" s="7"/>
+      <c r="L650" s="6"/>
     </row>
     <row r="651">
-      <c r="L651" s="7"/>
+      <c r="L651" s="6"/>
     </row>
     <row r="652">
-      <c r="L652" s="7"/>
+      <c r="L652" s="6"/>
     </row>
     <row r="653">
-      <c r="L653" s="7"/>
+      <c r="L653" s="6"/>
     </row>
     <row r="654">
-      <c r="L654" s="7"/>
+      <c r="L654" s="6"/>
     </row>
     <row r="655">
-      <c r="L655" s="7"/>
+      <c r="L655" s="6"/>
     </row>
     <row r="656">
-      <c r="L656" s="7"/>
+      <c r="L656" s="6"/>
     </row>
     <row r="657">
-      <c r="L657" s="7"/>
+      <c r="L657" s="6"/>
     </row>
     <row r="658">
-      <c r="L658" s="7"/>
+      <c r="L658" s="6"/>
     </row>
     <row r="659">
-      <c r="L659" s="7"/>
+      <c r="L659" s="6"/>
     </row>
     <row r="660">
-      <c r="L660" s="7"/>
+      <c r="L660" s="6"/>
     </row>
     <row r="661">
-      <c r="L661" s="7"/>
+      <c r="L661" s="6"/>
     </row>
     <row r="662">
-      <c r="L662" s="7"/>
+      <c r="L662" s="6"/>
     </row>
     <row r="663">
-      <c r="L663" s="7"/>
+      <c r="L663" s="6"/>
     </row>
     <row r="664">
-      <c r="L664" s="7"/>
+      <c r="L664" s="6"/>
     </row>
     <row r="665">
-      <c r="L665" s="7"/>
+      <c r="L665" s="6"/>
     </row>
     <row r="666">
-      <c r="L666" s="7"/>
+      <c r="L666" s="6"/>
     </row>
     <row r="667">
-      <c r="L667" s="7"/>
+      <c r="L667" s="6"/>
     </row>
     <row r="668">
-      <c r="L668" s="7"/>
+      <c r="L668" s="6"/>
     </row>
     <row r="669">
-      <c r="L669" s="7"/>
+      <c r="L669" s="6"/>
     </row>
     <row r="670">
-      <c r="L670" s="7"/>
+      <c r="L670" s="6"/>
     </row>
     <row r="671">
-      <c r="L671" s="7"/>
+      <c r="L671" s="6"/>
     </row>
     <row r="672">
-      <c r="L672" s="7"/>
+      <c r="L672" s="6"/>
     </row>
     <row r="673">
-      <c r="L673" s="7"/>
+      <c r="L673" s="6"/>
     </row>
     <row r="674">
-      <c r="L674" s="7"/>
+      <c r="L674" s="6"/>
     </row>
     <row r="675">
-      <c r="L675" s="7"/>
+      <c r="L675" s="6"/>
     </row>
     <row r="676">
-      <c r="L676" s="7"/>
+      <c r="L676" s="6"/>
     </row>
     <row r="677">
-      <c r="L677" s="7"/>
+      <c r="L677" s="6"/>
     </row>
     <row r="678">
-      <c r="L678" s="7"/>
+      <c r="L678" s="6"/>
     </row>
     <row r="679">
-      <c r="L679" s="7"/>
+      <c r="L679" s="6"/>
     </row>
     <row r="680">
-      <c r="L680" s="7"/>
+      <c r="L680" s="6"/>
     </row>
     <row r="681">
-      <c r="L681" s="7"/>
+      <c r="L681" s="6"/>
     </row>
     <row r="682">
-      <c r="L682" s="7"/>
+      <c r="L682" s="6"/>
     </row>
     <row r="683">
-      <c r="L683" s="7"/>
+      <c r="L683" s="6"/>
     </row>
     <row r="684">
-      <c r="L684" s="7"/>
+      <c r="L684" s="6"/>
     </row>
     <row r="685">
-      <c r="L685" s="7"/>
+      <c r="L685" s="6"/>
     </row>
     <row r="686">
-      <c r="L686" s="7"/>
+      <c r="L686" s="6"/>
     </row>
     <row r="687">
-      <c r="L687" s="7"/>
+      <c r="L687" s="6"/>
     </row>
     <row r="688">
-      <c r="L688" s="7"/>
+      <c r="L688" s="6"/>
     </row>
     <row r="689">
-      <c r="L689" s="7"/>
+      <c r="L689" s="6"/>
     </row>
     <row r="690">
-      <c r="L690" s="7"/>
+      <c r="L690" s="6"/>
     </row>
     <row r="691">
-      <c r="L691" s="7"/>
+      <c r="L691" s="6"/>
     </row>
     <row r="692">
-      <c r="L692" s="7"/>
+      <c r="L692" s="6"/>
     </row>
     <row r="693">
-      <c r="L693" s="7"/>
+      <c r="L693" s="6"/>
     </row>
     <row r="694">
-      <c r="L694" s="7"/>
+      <c r="L694" s="6"/>
     </row>
     <row r="695">
-      <c r="L695" s="7"/>
+      <c r="L695" s="6"/>
     </row>
     <row r="696">
-      <c r="L696" s="7"/>
+      <c r="L696" s="6"/>
     </row>
     <row r="697">
-      <c r="L697" s="7"/>
+      <c r="L697" s="6"/>
     </row>
     <row r="698">
-      <c r="L698" s="7"/>
+      <c r="L698" s="6"/>
     </row>
     <row r="699">
-      <c r="L699" s="7"/>
+      <c r="L699" s="6"/>
     </row>
     <row r="700">
-      <c r="L700" s="7"/>
+      <c r="L700" s="6"/>
     </row>
     <row r="701">
-      <c r="L701" s="7"/>
+      <c r="L701" s="6"/>
     </row>
     <row r="702">
-      <c r="L702" s="7"/>
+      <c r="L702" s="6"/>
     </row>
     <row r="703">
-      <c r="L703" s="7"/>
+      <c r="L703" s="6"/>
     </row>
     <row r="704">
-      <c r="L704" s="7"/>
+      <c r="L704" s="6"/>
     </row>
     <row r="705">
-      <c r="L705" s="7"/>
+      <c r="L705" s="6"/>
     </row>
     <row r="706">
-      <c r="L706" s="7"/>
+      <c r="L706" s="6"/>
     </row>
     <row r="707">
-      <c r="L707" s="7"/>
+      <c r="L707" s="6"/>
     </row>
     <row r="708">
-      <c r="L708" s="7"/>
+      <c r="L708" s="6"/>
     </row>
     <row r="709">
-      <c r="L709" s="7"/>
+      <c r="L709" s="6"/>
     </row>
     <row r="710">
-      <c r="L710" s="7"/>
+      <c r="L710" s="6"/>
     </row>
     <row r="711">
-      <c r="L711" s="7"/>
+      <c r="L711" s="6"/>
     </row>
     <row r="712">
-      <c r="L712" s="7"/>
+      <c r="L712" s="6"/>
     </row>
     <row r="713">
-      <c r="L713" s="7"/>
+      <c r="L713" s="6"/>
     </row>
     <row r="714">
-      <c r="L714" s="7"/>
+      <c r="L714" s="6"/>
     </row>
     <row r="715">
-      <c r="L715" s="7"/>
+      <c r="L715" s="6"/>
     </row>
     <row r="716">
-      <c r="L716" s="7"/>
+      <c r="L716" s="6"/>
     </row>
     <row r="717">
-      <c r="L717" s="7"/>
+      <c r="L717" s="6"/>
     </row>
     <row r="718">
-      <c r="L718" s="7"/>
+      <c r="L718" s="6"/>
     </row>
     <row r="719">
-      <c r="L719" s="7"/>
+      <c r="L719" s="6"/>
     </row>
     <row r="720">
-      <c r="L720" s="7"/>
+      <c r="L720" s="6"/>
     </row>
     <row r="721">
-      <c r="L721" s="7"/>
+      <c r="L721" s="6"/>
     </row>
     <row r="722">
-      <c r="L722" s="7"/>
+      <c r="L722" s="6"/>
     </row>
     <row r="723">
-      <c r="L723" s="7"/>
+      <c r="L723" s="6"/>
     </row>
     <row r="724">
-      <c r="L724" s="7"/>
+      <c r="L724" s="6"/>
     </row>
     <row r="725">
-      <c r="L725" s="7"/>
+      <c r="L725" s="6"/>
     </row>
     <row r="726">
-      <c r="L726" s="7"/>
+      <c r="L726" s="6"/>
     </row>
     <row r="727">
-      <c r="L727" s="7"/>
+      <c r="L727" s="6"/>
     </row>
     <row r="728">
-      <c r="L728" s="7"/>
+      <c r="L728" s="6"/>
     </row>
     <row r="729">
-      <c r="L729" s="7"/>
+      <c r="L729" s="6"/>
     </row>
     <row r="730">
-      <c r="L730" s="7"/>
+      <c r="L730" s="6"/>
     </row>
     <row r="731">
-      <c r="L731" s="7"/>
+      <c r="L731" s="6"/>
     </row>
     <row r="732">
-      <c r="L732" s="7"/>
+      <c r="L732" s="6"/>
     </row>
     <row r="733">
-      <c r="L733" s="7"/>
+      <c r="L733" s="6"/>
     </row>
     <row r="734">
-      <c r="L734" s="7"/>
+      <c r="L734" s="6"/>
     </row>
     <row r="735">
-      <c r="L735" s="7"/>
+      <c r="L735" s="6"/>
     </row>
     <row r="736">
-      <c r="L736" s="7"/>
+      <c r="L736" s="6"/>
     </row>
     <row r="737">
-      <c r="L737" s="7"/>
+      <c r="L737" s="6"/>
     </row>
     <row r="738">
-      <c r="L738" s="7"/>
+      <c r="L738" s="6"/>
     </row>
     <row r="739">
-      <c r="L739" s="7"/>
+      <c r="L739" s="6"/>
     </row>
     <row r="740">
-      <c r="L740" s="7"/>
+      <c r="L740" s="6"/>
     </row>
     <row r="741">
-      <c r="L741" s="7"/>
+      <c r="L741" s="6"/>
     </row>
     <row r="742">
-      <c r="L742" s="7"/>
+      <c r="L742" s="6"/>
     </row>
     <row r="743">
-      <c r="L743" s="7"/>
+      <c r="L743" s="6"/>
     </row>
     <row r="744">
-      <c r="L744" s="7"/>
+      <c r="L744" s="6"/>
     </row>
     <row r="745">
-      <c r="L745" s="7"/>
+      <c r="L745" s="6"/>
     </row>
     <row r="746">
-      <c r="L746" s="7"/>
+      <c r="L746" s="6"/>
     </row>
     <row r="747">
-      <c r="L747" s="7"/>
+      <c r="L747" s="6"/>
     </row>
     <row r="748">
-      <c r="L748" s="7"/>
+      <c r="L748" s="6"/>
     </row>
     <row r="749">
-      <c r="L749" s="7"/>
+      <c r="L749" s="6"/>
     </row>
     <row r="750">
-      <c r="L750" s="7"/>
+      <c r="L750" s="6"/>
     </row>
     <row r="751">
-      <c r="L751" s="7"/>
+      <c r="L751" s="6"/>
     </row>
     <row r="752">
-      <c r="L752" s="7"/>
+      <c r="L752" s="6"/>
     </row>
     <row r="753">
-      <c r="L753" s="7"/>
+      <c r="L753" s="6"/>
     </row>
     <row r="754">
-      <c r="L754" s="7"/>
+      <c r="L754" s="6"/>
     </row>
     <row r="755">
-      <c r="L755" s="7"/>
+      <c r="L755" s="6"/>
     </row>
     <row r="756">
-      <c r="L756" s="7"/>
+      <c r="L756" s="6"/>
     </row>
     <row r="757">
-      <c r="L757" s="7"/>
+      <c r="L757" s="6"/>
     </row>
     <row r="758">
-      <c r="L758" s="7"/>
+      <c r="L758" s="6"/>
     </row>
     <row r="759">
-      <c r="L759" s="7"/>
+      <c r="L759" s="6"/>
     </row>
     <row r="760">
-      <c r="L760" s="7"/>
+      <c r="L760" s="6"/>
     </row>
     <row r="761">
-      <c r="L761" s="7"/>
+      <c r="L761" s="6"/>
     </row>
     <row r="762">
-      <c r="L762" s="7"/>
+      <c r="L762" s="6"/>
     </row>
     <row r="763">
-      <c r="L763" s="7"/>
+      <c r="L763" s="6"/>
     </row>
     <row r="764">
-      <c r="L764" s="7"/>
+      <c r="L764" s="6"/>
     </row>
     <row r="765">
-      <c r="L765" s="7"/>
+      <c r="L765" s="6"/>
     </row>
     <row r="766">
-      <c r="L766" s="7"/>
+      <c r="L766" s="6"/>
     </row>
     <row r="767">
-      <c r="L767" s="7"/>
+      <c r="L767" s="6"/>
     </row>
     <row r="768">
-      <c r="L768" s="7"/>
+      <c r="L768" s="6"/>
     </row>
     <row r="769">
-      <c r="L769" s="7"/>
+      <c r="L769" s="6"/>
     </row>
     <row r="770">
-      <c r="L770" s="7"/>
+      <c r="L770" s="6"/>
     </row>
     <row r="771">
-      <c r="L771" s="7"/>
+      <c r="L771" s="6"/>
     </row>
     <row r="772">
-      <c r="L772" s="7"/>
+      <c r="L772" s="6"/>
     </row>
     <row r="773">
-      <c r="L773" s="7"/>
+      <c r="L773" s="6"/>
     </row>
     <row r="774">
-      <c r="L774" s="7"/>
+      <c r="L774" s="6"/>
     </row>
     <row r="775">
-      <c r="L775" s="7"/>
+      <c r="L775" s="6"/>
     </row>
     <row r="776">
-      <c r="L776" s="7"/>
+      <c r="L776" s="6"/>
     </row>
     <row r="777">
-      <c r="L777" s="7"/>
+      <c r="L777" s="6"/>
     </row>
     <row r="778">
-      <c r="L778" s="7"/>
+      <c r="L778" s="6"/>
     </row>
     <row r="779">
-      <c r="L779" s="7"/>
+      <c r="L779" s="6"/>
     </row>
     <row r="780">
-      <c r="L780" s="7"/>
+      <c r="L780" s="6"/>
     </row>
     <row r="781">
-      <c r="L781" s="7"/>
+      <c r="L781" s="6"/>
     </row>
     <row r="782">
-      <c r="L782" s="7"/>
+      <c r="L782" s="6"/>
     </row>
     <row r="783">
-      <c r="L783" s="7"/>
+      <c r="L783" s="6"/>
     </row>
     <row r="784">
-      <c r="L784" s="7"/>
+      <c r="L784" s="6"/>
     </row>
     <row r="785">
-      <c r="L785" s="7"/>
+      <c r="L785" s="6"/>
     </row>
     <row r="786">
-      <c r="L786" s="7"/>
+      <c r="L786" s="6"/>
     </row>
     <row r="787">
-      <c r="L787" s="7"/>
+      <c r="L787" s="6"/>
     </row>
     <row r="788">
-      <c r="L788" s="7"/>
+      <c r="L788" s="6"/>
     </row>
     <row r="789">
-      <c r="L789" s="7"/>
+      <c r="L789" s="6"/>
     </row>
     <row r="790">
-      <c r="L790" s="7"/>
+      <c r="L790" s="6"/>
     </row>
     <row r="791">
-      <c r="L791" s="7"/>
+      <c r="L791" s="6"/>
     </row>
     <row r="792">
-      <c r="L792" s="7"/>
+      <c r="L792" s="6"/>
     </row>
     <row r="793">
-      <c r="L793" s="7"/>
+      <c r="L793" s="6"/>
     </row>
     <row r="794">
-      <c r="L794" s="7"/>
+      <c r="L794" s="6"/>
     </row>
     <row r="795">
-      <c r="L795" s="7"/>
+      <c r="L795" s="6"/>
     </row>
     <row r="796">
-      <c r="L796" s="7"/>
+      <c r="L796" s="6"/>
     </row>
     <row r="797">
-      <c r="L797" s="7"/>
+      <c r="L797" s="6"/>
     </row>
     <row r="798">
-      <c r="L798" s="7"/>
+      <c r="L798" s="6"/>
     </row>
     <row r="799">
-      <c r="L799" s="7"/>
+      <c r="L799" s="6"/>
     </row>
     <row r="800">
-      <c r="L800" s="7"/>
+      <c r="L800" s="6"/>
     </row>
     <row r="801">
-      <c r="L801" s="7"/>
+      <c r="L801" s="6"/>
     </row>
     <row r="802">
-      <c r="L802" s="7"/>
+      <c r="L802" s="6"/>
     </row>
     <row r="803">
-      <c r="L803" s="7"/>
+      <c r="L803" s="6"/>
     </row>
     <row r="804">
-      <c r="L804" s="7"/>
+      <c r="L804" s="6"/>
     </row>
     <row r="805">
-      <c r="L805" s="7"/>
+      <c r="L805" s="6"/>
     </row>
     <row r="806">
-      <c r="L806" s="7"/>
+      <c r="L806" s="6"/>
     </row>
     <row r="807">
-      <c r="L807" s="7"/>
+      <c r="L807" s="6"/>
     </row>
     <row r="808">
-      <c r="L808" s="7"/>
+      <c r="L808" s="6"/>
     </row>
     <row r="809">
-      <c r="L809" s="7"/>
+      <c r="L809" s="6"/>
     </row>
     <row r="810">
-      <c r="L810" s="7"/>
+      <c r="L810" s="6"/>
     </row>
     <row r="811">
-      <c r="L811" s="7"/>
+      <c r="L811" s="6"/>
     </row>
     <row r="812">
-      <c r="L812" s="7"/>
+      <c r="L812" s="6"/>
     </row>
     <row r="813">
-      <c r="L813" s="7"/>
+      <c r="L813" s="6"/>
     </row>
     <row r="814">
-      <c r="L814" s="7"/>
+      <c r="L814" s="6"/>
     </row>
     <row r="815">
-      <c r="L815" s="7"/>
+      <c r="L815" s="6"/>
     </row>
     <row r="816">
-      <c r="L816" s="7"/>
+      <c r="L816" s="6"/>
     </row>
     <row r="817">
-      <c r="L817" s="7"/>
+      <c r="L817" s="6"/>
     </row>
     <row r="818">
-      <c r="L818" s="7"/>
+      <c r="L818" s="6"/>
     </row>
     <row r="819">
-      <c r="L819" s="7"/>
+      <c r="L819" s="6"/>
     </row>
     <row r="820">
-      <c r="L820" s="7"/>
+      <c r="L820" s="6"/>
     </row>
     <row r="821">
-      <c r="L821" s="7"/>
+      <c r="L821" s="6"/>
     </row>
     <row r="822">
-      <c r="L822" s="7"/>
+      <c r="L822" s="6"/>
     </row>
     <row r="823">
-      <c r="L823" s="7"/>
+      <c r="L823" s="6"/>
     </row>
     <row r="824">
-      <c r="L824" s="7"/>
+      <c r="L824" s="6"/>
     </row>
     <row r="825">
-      <c r="L825" s="7"/>
+      <c r="L825" s="6"/>
     </row>
     <row r="826">
-      <c r="L826" s="7"/>
+      <c r="L826" s="6"/>
     </row>
     <row r="827">
-      <c r="L827" s="7"/>
+      <c r="L827" s="6"/>
     </row>
     <row r="828">
-      <c r="L828" s="7"/>
+      <c r="L828" s="6"/>
     </row>
     <row r="829">
-      <c r="L829" s="7"/>
+      <c r="L829" s="6"/>
     </row>
     <row r="830">
-      <c r="L830" s="7"/>
+      <c r="L830" s="6"/>
     </row>
     <row r="831">
-      <c r="L831" s="7"/>
+      <c r="L831" s="6"/>
     </row>
     <row r="832">
-      <c r="L832" s="7"/>
+      <c r="L832" s="6"/>
     </row>
     <row r="833">
-      <c r="L833" s="7"/>
+      <c r="L833" s="6"/>
     </row>
     <row r="834">
-      <c r="L834" s="7"/>
+      <c r="L834" s="6"/>
     </row>
     <row r="835">
-      <c r="L835" s="7"/>
+      <c r="L835" s="6"/>
     </row>
     <row r="836">
-      <c r="L836" s="7"/>
+      <c r="L836" s="6"/>
     </row>
     <row r="837">
-      <c r="L837" s="7"/>
+      <c r="L837" s="6"/>
     </row>
     <row r="838">
-      <c r="L838" s="7"/>
+      <c r="L838" s="6"/>
     </row>
     <row r="839">
-      <c r="L839" s="7"/>
+      <c r="L839" s="6"/>
     </row>
     <row r="840">
-      <c r="L840" s="7"/>
+      <c r="L840" s="6"/>
     </row>
     <row r="841">
-      <c r="L841" s="7"/>
+      <c r="L841" s="6"/>
     </row>
     <row r="842">
-      <c r="L842" s="7"/>
+      <c r="L842" s="6"/>
     </row>
     <row r="843">
-      <c r="L843" s="7"/>
+      <c r="L843" s="6"/>
     </row>
     <row r="844">
-      <c r="L844" s="7"/>
+      <c r="L844" s="6"/>
     </row>
     <row r="845">
-      <c r="L845" s="7"/>
+      <c r="L845" s="6"/>
     </row>
     <row r="846">
-      <c r="L846" s="7"/>
+      <c r="L846" s="6"/>
     </row>
     <row r="847">
-      <c r="L847" s="7"/>
+      <c r="L847" s="6"/>
     </row>
     <row r="848">
-      <c r="L848" s="7"/>
+      <c r="L848" s="6"/>
     </row>
     <row r="849">
-      <c r="L849" s="7"/>
+      <c r="L849" s="6"/>
     </row>
     <row r="850">
-      <c r="L850" s="7"/>
+      <c r="L850" s="6"/>
     </row>
     <row r="851">
-      <c r="L851" s="7"/>
+      <c r="L851" s="6"/>
     </row>
     <row r="852">
-      <c r="L852" s="7"/>
+      <c r="L852" s="6"/>
     </row>
     <row r="853">
-      <c r="L853" s="7"/>
+      <c r="L853" s="6"/>
     </row>
     <row r="854">
-      <c r="L854" s="7"/>
+      <c r="L854" s="6"/>
     </row>
     <row r="855">
-      <c r="L855" s="7"/>
+      <c r="L855" s="6"/>
     </row>
     <row r="856">
-      <c r="L856" s="7"/>
+      <c r="L856" s="6"/>
     </row>
     <row r="857">
-      <c r="L857" s="7"/>
+      <c r="L857" s="6"/>
     </row>
     <row r="858">
-      <c r="L858" s="7"/>
+      <c r="L858" s="6"/>
     </row>
     <row r="859">
-      <c r="L859" s="7"/>
+      <c r="L859" s="6"/>
     </row>
     <row r="860">
-      <c r="L860" s="7"/>
+      <c r="L860" s="6"/>
     </row>
     <row r="861">
-      <c r="L861" s="7"/>
+      <c r="L861" s="6"/>
     </row>
     <row r="862">
-      <c r="L862" s="7"/>
+      <c r="L862" s="6"/>
     </row>
     <row r="863">
-      <c r="L863" s="7"/>
+      <c r="L863" s="6"/>
     </row>
     <row r="864">
-      <c r="L864" s="7"/>
+      <c r="L864" s="6"/>
     </row>
     <row r="865">
-      <c r="L865" s="7"/>
+      <c r="L865" s="6"/>
     </row>
     <row r="866">
-      <c r="L866" s="7"/>
+      <c r="L866" s="6"/>
     </row>
     <row r="867">
-      <c r="L867" s="7"/>
+      <c r="L867" s="6"/>
     </row>
     <row r="868">
-      <c r="L868" s="7"/>
+      <c r="L868" s="6"/>
     </row>
     <row r="869">
-      <c r="L869" s="7"/>
+      <c r="L869" s="6"/>
     </row>
     <row r="870">
-      <c r="L870" s="7"/>
+      <c r="L870" s="6"/>
     </row>
     <row r="871">
-      <c r="L871" s="7"/>
+      <c r="L871" s="6"/>
     </row>
     <row r="872">
-      <c r="L872" s="7"/>
+      <c r="L872" s="6"/>
     </row>
     <row r="873">
-      <c r="L873" s="7"/>
+      <c r="L873" s="6"/>
     </row>
     <row r="874">
-      <c r="L874" s="7"/>
+      <c r="L874" s="6"/>
     </row>
     <row r="875">
-      <c r="L875" s="7"/>
+      <c r="L875" s="6"/>
     </row>
     <row r="876">
-      <c r="L876" s="7"/>
+      <c r="L876" s="6"/>
     </row>
     <row r="877">
-      <c r="L877" s="7"/>
+      <c r="L877" s="6"/>
     </row>
     <row r="878">
-      <c r="L878" s="7"/>
+      <c r="L878" s="6"/>
     </row>
     <row r="879">
-      <c r="L879" s="7"/>
+      <c r="L879" s="6"/>
     </row>
     <row r="880">
-      <c r="L880" s="7"/>
+      <c r="L880" s="6"/>
     </row>
     <row r="881">
-      <c r="L881" s="7"/>
+      <c r="L881" s="6"/>
     </row>
     <row r="882">
-      <c r="L882" s="7"/>
+      <c r="L882" s="6"/>
     </row>
     <row r="883">
-      <c r="L883" s="7"/>
+      <c r="L883" s="6"/>
     </row>
     <row r="884">
-      <c r="L884" s="7"/>
+      <c r="L884" s="6"/>
     </row>
     <row r="885">
-      <c r="L885" s="7"/>
+      <c r="L885" s="6"/>
     </row>
     <row r="886">
-      <c r="L886" s="7"/>
+      <c r="L886" s="6"/>
     </row>
     <row r="887">
-      <c r="L887" s="7"/>
+      <c r="L887" s="6"/>
     </row>
     <row r="888">
-      <c r="L888" s="7"/>
+      <c r="L888" s="6"/>
     </row>
     <row r="889">
-      <c r="L889" s="7"/>
+      <c r="L889" s="6"/>
     </row>
     <row r="890">
-      <c r="L890" s="7"/>
+      <c r="L890" s="6"/>
     </row>
     <row r="891">
-      <c r="L891" s="7"/>
+      <c r="L891" s="6"/>
     </row>
     <row r="892">
-      <c r="L892" s="7"/>
+      <c r="L892" s="6"/>
     </row>
     <row r="893">
-      <c r="L893" s="7"/>
+      <c r="L893" s="6"/>
     </row>
     <row r="894">
-      <c r="L894" s="7"/>
+      <c r="L894" s="6"/>
     </row>
     <row r="895">
-      <c r="L895" s="7"/>
+      <c r="L895" s="6"/>
     </row>
     <row r="896">
-      <c r="L896" s="7"/>
+      <c r="L896" s="6"/>
     </row>
     <row r="897">
-      <c r="L897" s="7"/>
+      <c r="L897" s="6"/>
     </row>
     <row r="898">
-      <c r="L898" s="7"/>
+      <c r="L898" s="6"/>
     </row>
     <row r="899">
-      <c r="L899" s="7"/>
+      <c r="L899" s="6"/>
     </row>
     <row r="900">
-      <c r="L900" s="7"/>
+      <c r="L900" s="6"/>
     </row>
     <row r="901">
-      <c r="L901" s="7"/>
+      <c r="L901" s="6"/>
     </row>
     <row r="902">
-      <c r="L902" s="7"/>
+      <c r="L902" s="6"/>
     </row>
     <row r="903">
-      <c r="L903" s="7"/>
+      <c r="L903" s="6"/>
     </row>
     <row r="904">
-      <c r="L904" s="7"/>
+      <c r="L904" s="6"/>
     </row>
     <row r="905">
-      <c r="L905" s="7"/>
+      <c r="L905" s="6"/>
     </row>
     <row r="906">
-      <c r="L906" s="7"/>
+      <c r="L906" s="6"/>
     </row>
     <row r="907">
-      <c r="L907" s="7"/>
+      <c r="L907" s="6"/>
     </row>
     <row r="908">
-      <c r="L908" s="7"/>
+      <c r="L908" s="6"/>
     </row>
     <row r="909">
-      <c r="L909" s="7"/>
+      <c r="L909" s="6"/>
     </row>
     <row r="910">
-      <c r="L910" s="7"/>
+      <c r="L910" s="6"/>
     </row>
     <row r="911">
-      <c r="L911" s="7"/>
+      <c r="L911" s="6"/>
     </row>
     <row r="912">
-      <c r="L912" s="7"/>
+      <c r="L912" s="6"/>
     </row>
     <row r="913">
-      <c r="L913" s="7"/>
+      <c r="L913" s="6"/>
     </row>
     <row r="914">
-      <c r="L914" s="7"/>
+      <c r="L914" s="6"/>
     </row>
     <row r="915">
-      <c r="L915" s="7"/>
+      <c r="L915" s="6"/>
     </row>
     <row r="916">
-      <c r="L916" s="7"/>
+      <c r="L916" s="6"/>
     </row>
     <row r="917">
-      <c r="L917" s="7"/>
+      <c r="L917" s="6"/>
     </row>
     <row r="918">
-      <c r="L918" s="7"/>
+      <c r="L918" s="6"/>
     </row>
     <row r="919">
-      <c r="L919" s="7"/>
+      <c r="L919" s="6"/>
     </row>
     <row r="920">
-      <c r="L920" s="7"/>
+      <c r="L920" s="6"/>
     </row>
     <row r="921">
-      <c r="L921" s="7"/>
+      <c r="L921" s="6"/>
     </row>
     <row r="922">
-      <c r="L922" s="7"/>
+      <c r="L922" s="6"/>
     </row>
     <row r="923">
-      <c r="L923" s="7"/>
+      <c r="L923" s="6"/>
     </row>
     <row r="924">
-      <c r="L924" s="7"/>
+      <c r="L924" s="6"/>
     </row>
     <row r="925">
-      <c r="L925" s="7"/>
+      <c r="L925" s="6"/>
     </row>
     <row r="926">
-      <c r="L926" s="7"/>
+      <c r="L926" s="6"/>
     </row>
     <row r="927">
-      <c r="L927" s="7"/>
+      <c r="L927" s="6"/>
     </row>
     <row r="928">
-      <c r="L928" s="7"/>
+      <c r="L928" s="6"/>
     </row>
     <row r="929">
-      <c r="L929" s="7"/>
+      <c r="L929" s="6"/>
     </row>
     <row r="930">
-      <c r="L930" s="7"/>
+      <c r="L930" s="6"/>
     </row>
     <row r="931">
-      <c r="L931" s="7"/>
+      <c r="L931" s="6"/>
     </row>
     <row r="932">
-      <c r="L932" s="7"/>
+      <c r="L932" s="6"/>
     </row>
     <row r="933">
-      <c r="L933" s="7"/>
+      <c r="L933" s="6"/>
     </row>
     <row r="934">
-      <c r="L934" s="7"/>
+      <c r="L934" s="6"/>
     </row>
     <row r="935">
-      <c r="L935" s="7"/>
+      <c r="L935" s="6"/>
     </row>
     <row r="936">
-      <c r="L936" s="7"/>
+      <c r="L936" s="6"/>
     </row>
     <row r="937">
-      <c r="L937" s="7"/>
+      <c r="L937" s="6"/>
     </row>
     <row r="938">
-      <c r="L938" s="7"/>
+      <c r="L938" s="6"/>
     </row>
     <row r="939">
-      <c r="L939" s="7"/>
+      <c r="L939" s="6"/>
     </row>
     <row r="940">
-      <c r="L940" s="7"/>
+      <c r="L940" s="6"/>
     </row>
     <row r="941">
-      <c r="L941" s="7"/>
+      <c r="L941" s="6"/>
     </row>
     <row r="942">
-      <c r="L942" s="7"/>
+      <c r="L942" s="6"/>
     </row>
     <row r="943">
-      <c r="L943" s="7"/>
+      <c r="L943" s="6"/>
     </row>
     <row r="944">
-      <c r="L944" s="7"/>
+      <c r="L944" s="6"/>
     </row>
     <row r="945">
-      <c r="L945" s="7"/>
+      <c r="L945" s="6"/>
     </row>
     <row r="946">
-      <c r="L946" s="7"/>
+      <c r="L946" s="6"/>
     </row>
     <row r="947">
-      <c r="L947" s="7"/>
+      <c r="L947" s="6"/>
     </row>
     <row r="948">
-      <c r="L948" s="7"/>
+      <c r="L948" s="6"/>
     </row>
     <row r="949">
-      <c r="L949" s="7"/>
+      <c r="L949" s="6"/>
     </row>
     <row r="950">
-      <c r="L950" s="7"/>
+      <c r="L950" s="6"/>
     </row>
     <row r="951">
-      <c r="L951" s="7"/>
+      <c r="L951" s="6"/>
     </row>
     <row r="952">
-      <c r="L952" s="7"/>
+      <c r="L952" s="6"/>
     </row>
     <row r="953">
-      <c r="L953" s="7"/>
+      <c r="L953" s="6"/>
     </row>
     <row r="954">
-      <c r="L954" s="7"/>
+      <c r="L954" s="6"/>
     </row>
     <row r="955">
-      <c r="L955" s="7"/>
+      <c r="L955" s="6"/>
     </row>
     <row r="956">
-      <c r="L956" s="7"/>
+      <c r="L956" s="6"/>
     </row>
     <row r="957">
-      <c r="L957" s="7"/>
+      <c r="L957" s="6"/>
     </row>
     <row r="958">
-      <c r="L958" s="7"/>
+      <c r="L958" s="6"/>
     </row>
     <row r="959">
-      <c r="L959" s="7"/>
+      <c r="L959" s="6"/>
     </row>
     <row r="960">
-      <c r="L960" s="7"/>
+      <c r="L960" s="6"/>
     </row>
     <row r="961">
-      <c r="L961" s="7"/>
+      <c r="L961" s="6"/>
     </row>
     <row r="962">
-      <c r="L962" s="7"/>
+      <c r="L962" s="6"/>
     </row>
     <row r="963">
-      <c r="L963" s="7"/>
+      <c r="L963" s="6"/>
     </row>
     <row r="964">
-      <c r="L964" s="7"/>
+      <c r="L964" s="6"/>
     </row>
     <row r="965">
-      <c r="L965" s="7"/>
+      <c r="L965" s="6"/>
     </row>
     <row r="966">
-      <c r="L966" s="7"/>
+      <c r="L966" s="6"/>
     </row>
     <row r="967">
-      <c r="L967" s="7"/>
+      <c r="L967" s="6"/>
     </row>
     <row r="968">
-      <c r="L968" s="7"/>
+      <c r="L968" s="6"/>
     </row>
     <row r="969">
-      <c r="L969" s="7"/>
+      <c r="L969" s="6"/>
     </row>
     <row r="970">
-      <c r="L970" s="7"/>
+      <c r="L970" s="6"/>
     </row>
     <row r="971">
-      <c r="L971" s="7"/>
+      <c r="L971" s="6"/>
     </row>
     <row r="972">
-      <c r="L972" s="7"/>
+      <c r="L972" s="6"/>
     </row>
     <row r="973">
-      <c r="L973" s="7"/>
+      <c r="L973" s="6"/>
     </row>
     <row r="974">
-      <c r="L974" s="7"/>
+      <c r="L974" s="6"/>
     </row>
     <row r="975">
-      <c r="L975" s="7"/>
+      <c r="L975" s="6"/>
     </row>
     <row r="976">
-      <c r="L976" s="7"/>
+      <c r="L976" s="6"/>
     </row>
     <row r="977">
-      <c r="L977" s="7"/>
+      <c r="L977" s="6"/>
     </row>
     <row r="978">
-      <c r="L978" s="7"/>
+      <c r="L978" s="6"/>
     </row>
     <row r="979">
-      <c r="L979" s="7"/>
+      <c r="L979" s="6"/>
     </row>
     <row r="980">
-      <c r="L980" s="7"/>
+      <c r="L980" s="6"/>
     </row>
     <row r="981">
-      <c r="L981" s="7"/>
+      <c r="L981" s="6"/>
     </row>
     <row r="982">
-      <c r="L982" s="7"/>
+      <c r="L982" s="6"/>
     </row>
     <row r="983">
-      <c r="L983" s="7"/>
+      <c r="L983" s="6"/>
     </row>
     <row r="984">
-      <c r="L984" s="7"/>
+      <c r="L984" s="6"/>
     </row>
     <row r="985">
-      <c r="L985" s="7"/>
+      <c r="L985" s="6"/>
     </row>
     <row r="986">
-      <c r="L986" s="7"/>
+      <c r="L986" s="6"/>
     </row>
     <row r="987">
-      <c r="L987" s="7"/>
+      <c r="L987" s="6"/>
     </row>
     <row r="988">
-      <c r="L988" s="7"/>
+      <c r="L988" s="6"/>
     </row>
     <row r="989">
-      <c r="L989" s="7"/>
+      <c r="L989" s="6"/>
     </row>
     <row r="990">
-      <c r="L990" s="7"/>
+      <c r="L990" s="6"/>
     </row>
     <row r="991">
-      <c r="L991" s="7"/>
+      <c r="L991" s="6"/>
     </row>
     <row r="992">
-      <c r="L992" s="7"/>
+      <c r="L992" s="6"/>
     </row>
     <row r="993">
-      <c r="L993" s="7"/>
+      <c r="L993" s="6"/>
     </row>
     <row r="994">
-      <c r="L994" s="7"/>
+      <c r="L994" s="6"/>
     </row>
     <row r="995">
-      <c r="L995" s="7"/>
+      <c r="L995" s="6"/>
     </row>
     <row r="996">
-      <c r="L996" s="7"/>
+      <c r="L996" s="6"/>
     </row>
     <row r="997">
-      <c r="L997" s="7"/>
+      <c r="L997" s="6"/>
     </row>
     <row r="998">
-      <c r="L998" s="7"/>
+      <c r="L998" s="6"/>
     </row>
     <row r="999">
-      <c r="L999" s="7"/>
+      <c r="L999" s="6"/>
     </row>
     <row r="1000">
-      <c r="L1000" s="7"/>
+      <c r="L1000" s="6"/>
     </row>
   </sheetData>
   <drawing r:id="rId1"/>

</xml_diff>